<commit_message>
Update Direccion SIMAT 2004
</commit_message>
<xml_diff>
--- a/data/metadata/dicts/processed_SIMAT_2004_2022.xlsx
+++ b/data/metadata/dicts/processed_SIMAT_2004_2022.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="423">
   <si>
     <t xml:space="preserve">uniname</t>
   </si>
@@ -123,12 +123,12 @@
     <t xml:space="preserve">TIPO_DOCUMENTO</t>
   </si>
   <si>
+    <t xml:space="preserve">DIRECCION_RESIDENCIA</t>
+  </si>
+  <si>
     <t xml:space="preserve">GENERO</t>
   </si>
   <si>
-    <t xml:space="preserve">DIRECCION_RESIDENCIA</t>
-  </si>
-  <si>
     <t xml:space="preserve">ESTRATO</t>
   </si>
   <si>
@@ -895,9 +895,6 @@
   </si>
   <si>
     <t xml:space="preserve">DIF_EDAD MARZO...65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIREC_RESID</t>
   </si>
   <si>
     <t xml:space="preserve">DIRECCION_RESIDENCIA  HOMOLOGADA</t>
@@ -2396,7 +2393,7 @@
         <v>26</v>
       </c>
       <c r="E11" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
         <v>37</v>
@@ -2414,7 +2411,9 @@
       <c r="K11" t="s">
         <v>37</v>
       </c>
-      <c r="L11"/>
+      <c r="L11" t="s">
+        <v>37</v>
+      </c>
       <c r="M11" t="s">
         <v>37</v>
       </c>
@@ -13708,16 +13707,16 @@
       <c r="I259"/>
       <c r="J259"/>
       <c r="K259"/>
-      <c r="L259" t="s">
-        <v>294</v>
-      </c>
+      <c r="L259"/>
       <c r="M259"/>
       <c r="N259"/>
       <c r="O259"/>
       <c r="P259"/>
       <c r="Q259"/>
       <c r="R259"/>
-      <c r="S259"/>
+      <c r="S259" t="s">
+        <v>294</v>
+      </c>
       <c r="T259"/>
       <c r="U259"/>
       <c r="V259"/>
@@ -13730,13 +13729,13 @@
         <v>295</v>
       </c>
       <c r="B260" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C260" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D260" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E260" t="n">
         <v>5</v>
@@ -13754,14 +13753,14 @@
       <c r="P260"/>
       <c r="Q260"/>
       <c r="R260"/>
-      <c r="S260" t="s">
-        <v>295</v>
-      </c>
+      <c r="S260"/>
       <c r="T260"/>
       <c r="U260"/>
       <c r="V260"/>
       <c r="W260"/>
-      <c r="X260"/>
+      <c r="X260" t="s">
+        <v>295</v>
+      </c>
       <c r="Y260"/>
     </row>
     <row r="261">
@@ -13769,20 +13768,22 @@
         <v>296</v>
       </c>
       <c r="B261" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C261" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D261" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E261" t="n">
         <v>5</v>
       </c>
       <c r="F261"/>
       <c r="G261"/>
-      <c r="H261"/>
+      <c r="H261" t="s">
+        <v>296</v>
+      </c>
       <c r="I261"/>
       <c r="J261"/>
       <c r="K261"/>
@@ -13798,9 +13799,7 @@
       <c r="U261"/>
       <c r="V261"/>
       <c r="W261"/>
-      <c r="X261" t="s">
-        <v>296</v>
-      </c>
+      <c r="X261"/>
       <c r="Y261"/>
     </row>
     <row r="262">
@@ -13808,13 +13807,13 @@
         <v>297</v>
       </c>
       <c r="B262" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="C262" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="D262" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="E262" t="n">
         <v>5</v>
@@ -13847,13 +13846,13 @@
         <v>298</v>
       </c>
       <c r="B263" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="C263" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="D263" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="E263" t="n">
         <v>5</v>
@@ -13886,22 +13885,20 @@
         <v>299</v>
       </c>
       <c r="B264" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C264" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D264" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E264" t="n">
         <v>5</v>
       </c>
       <c r="F264"/>
       <c r="G264"/>
-      <c r="H264" t="s">
-        <v>299</v>
-      </c>
+      <c r="H264"/>
       <c r="I264"/>
       <c r="J264"/>
       <c r="K264"/>
@@ -13910,7 +13907,9 @@
       <c r="N264"/>
       <c r="O264"/>
       <c r="P264"/>
-      <c r="Q264"/>
+      <c r="Q264" t="s">
+        <v>299</v>
+      </c>
       <c r="R264"/>
       <c r="S264"/>
       <c r="T264"/>
@@ -13943,13 +13942,13 @@
       <c r="J265"/>
       <c r="K265"/>
       <c r="L265"/>
-      <c r="M265"/>
+      <c r="M265" t="s">
+        <v>300</v>
+      </c>
       <c r="N265"/>
       <c r="O265"/>
       <c r="P265"/>
-      <c r="Q265" t="s">
-        <v>300</v>
-      </c>
+      <c r="Q265"/>
       <c r="R265"/>
       <c r="S265"/>
       <c r="T265"/>
@@ -13980,11 +13979,11 @@
       <c r="H266"/>
       <c r="I266"/>
       <c r="J266"/>
-      <c r="K266"/>
+      <c r="K266" t="s">
+        <v>301</v>
+      </c>
       <c r="L266"/>
-      <c r="M266" t="s">
-        <v>301</v>
-      </c>
+      <c r="M266"/>
       <c r="N266"/>
       <c r="O266"/>
       <c r="P266"/>
@@ -14019,16 +14018,16 @@
       <c r="H267"/>
       <c r="I267"/>
       <c r="J267"/>
-      <c r="K267" t="s">
-        <v>302</v>
-      </c>
+      <c r="K267"/>
       <c r="L267"/>
       <c r="M267"/>
       <c r="N267"/>
       <c r="O267"/>
       <c r="P267"/>
       <c r="Q267"/>
-      <c r="R267"/>
+      <c r="R267" t="s">
+        <v>302</v>
+      </c>
       <c r="S267"/>
       <c r="T267"/>
       <c r="U267"/>
@@ -14065,10 +14064,10 @@
       <c r="O268"/>
       <c r="P268"/>
       <c r="Q268"/>
-      <c r="R268" t="s">
+      <c r="R268"/>
+      <c r="S268" t="s">
         <v>303</v>
       </c>
-      <c r="S268"/>
       <c r="T268"/>
       <c r="U268"/>
       <c r="V268"/>
@@ -14100,14 +14099,14 @@
       <c r="K269"/>
       <c r="L269"/>
       <c r="M269"/>
-      <c r="N269"/>
+      <c r="N269" t="s">
+        <v>304</v>
+      </c>
       <c r="O269"/>
       <c r="P269"/>
       <c r="Q269"/>
       <c r="R269"/>
-      <c r="S269" t="s">
-        <v>304</v>
-      </c>
+      <c r="S269"/>
       <c r="T269"/>
       <c r="U269"/>
       <c r="V269"/>
@@ -14215,11 +14214,11 @@
       <c r="I272"/>
       <c r="J272"/>
       <c r="K272"/>
-      <c r="L272"/>
+      <c r="L272" t="s">
+        <v>307</v>
+      </c>
       <c r="M272"/>
-      <c r="N272" t="s">
-        <v>307</v>
-      </c>
+      <c r="N272"/>
       <c r="O272"/>
       <c r="P272"/>
       <c r="Q272"/>
@@ -14254,11 +14253,11 @@
       <c r="I273"/>
       <c r="J273"/>
       <c r="K273"/>
-      <c r="L273" t="s">
+      <c r="L273"/>
+      <c r="M273"/>
+      <c r="N273" t="s">
         <v>308</v>
       </c>
-      <c r="M273"/>
-      <c r="N273"/>
       <c r="O273"/>
       <c r="P273"/>
       <c r="Q273"/>
@@ -14293,11 +14292,11 @@
       <c r="I274"/>
       <c r="J274"/>
       <c r="K274"/>
-      <c r="L274"/>
+      <c r="L274" t="s">
+        <v>309</v>
+      </c>
       <c r="M274"/>
-      <c r="N274" t="s">
-        <v>309</v>
-      </c>
+      <c r="N274"/>
       <c r="O274"/>
       <c r="P274"/>
       <c r="Q274"/>
@@ -14332,16 +14331,16 @@
       <c r="I275"/>
       <c r="J275"/>
       <c r="K275"/>
-      <c r="L275" t="s">
-        <v>310</v>
-      </c>
+      <c r="L275"/>
       <c r="M275"/>
       <c r="N275"/>
       <c r="O275"/>
       <c r="P275"/>
       <c r="Q275"/>
       <c r="R275"/>
-      <c r="S275"/>
+      <c r="S275" t="s">
+        <v>310</v>
+      </c>
       <c r="T275"/>
       <c r="U275"/>
       <c r="V275"/>
@@ -14377,10 +14376,10 @@
       <c r="O276"/>
       <c r="P276"/>
       <c r="Q276"/>
-      <c r="R276"/>
-      <c r="S276" t="s">
+      <c r="R276" t="s">
         <v>311</v>
       </c>
+      <c r="S276"/>
       <c r="T276"/>
       <c r="U276"/>
       <c r="V276"/>
@@ -14393,20 +14392,22 @@
         <v>312</v>
       </c>
       <c r="B277" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C277" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D277" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E277" t="n">
         <v>5</v>
       </c>
       <c r="F277"/>
       <c r="G277"/>
-      <c r="H277"/>
+      <c r="H277" t="s">
+        <v>312</v>
+      </c>
       <c r="I277"/>
       <c r="J277"/>
       <c r="K277"/>
@@ -14416,9 +14417,7 @@
       <c r="O277"/>
       <c r="P277"/>
       <c r="Q277"/>
-      <c r="R277" t="s">
-        <v>312</v>
-      </c>
+      <c r="R277"/>
       <c r="S277"/>
       <c r="T277"/>
       <c r="U277"/>
@@ -14484,9 +14483,7 @@
       </c>
       <c r="F279"/>
       <c r="G279"/>
-      <c r="H279" t="s">
-        <v>314</v>
-      </c>
+      <c r="H279"/>
       <c r="I279"/>
       <c r="J279"/>
       <c r="K279"/>
@@ -14497,7 +14494,9 @@
       <c r="P279"/>
       <c r="Q279"/>
       <c r="R279"/>
-      <c r="S279"/>
+      <c r="S279" t="s">
+        <v>314</v>
+      </c>
       <c r="T279"/>
       <c r="U279"/>
       <c r="V279"/>
@@ -14533,10 +14532,10 @@
       <c r="O280"/>
       <c r="P280"/>
       <c r="Q280"/>
-      <c r="R280"/>
-      <c r="S280" t="s">
+      <c r="R280" t="s">
         <v>315</v>
       </c>
+      <c r="S280"/>
       <c r="T280"/>
       <c r="U280"/>
       <c r="V280"/>
@@ -14571,10 +14570,10 @@
       <c r="N281"/>
       <c r="O281"/>
       <c r="P281"/>
-      <c r="Q281"/>
-      <c r="R281" t="s">
+      <c r="Q281" t="s">
         <v>316</v>
       </c>
+      <c r="R281"/>
       <c r="S281"/>
       <c r="T281"/>
       <c r="U281"/>
@@ -14644,14 +14643,14 @@
       <c r="I283"/>
       <c r="J283"/>
       <c r="K283"/>
-      <c r="L283"/>
+      <c r="L283" t="s">
+        <v>318</v>
+      </c>
       <c r="M283"/>
       <c r="N283"/>
       <c r="O283"/>
       <c r="P283"/>
-      <c r="Q283" t="s">
-        <v>318</v>
-      </c>
+      <c r="Q283"/>
       <c r="R283"/>
       <c r="S283"/>
       <c r="T283"/>
@@ -14666,13 +14665,13 @@
         <v>319</v>
       </c>
       <c r="B284" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C284" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D284" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E284" t="n">
         <v>5</v>
@@ -14683,16 +14682,16 @@
       <c r="I284"/>
       <c r="J284"/>
       <c r="K284"/>
-      <c r="L284" t="s">
-        <v>319</v>
-      </c>
+      <c r="L284"/>
       <c r="M284"/>
       <c r="N284"/>
       <c r="O284"/>
       <c r="P284"/>
       <c r="Q284"/>
       <c r="R284"/>
-      <c r="S284"/>
+      <c r="S284" t="s">
+        <v>319</v>
+      </c>
       <c r="T284"/>
       <c r="U284"/>
       <c r="V284"/>
@@ -14705,13 +14704,13 @@
         <v>320</v>
       </c>
       <c r="B285" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C285" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D285" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E285" t="n">
         <v>5</v>
@@ -14720,7 +14719,9 @@
       <c r="G285"/>
       <c r="H285"/>
       <c r="I285"/>
-      <c r="J285"/>
+      <c r="J285" t="s">
+        <v>320</v>
+      </c>
       <c r="K285"/>
       <c r="L285"/>
       <c r="M285"/>
@@ -14729,9 +14730,7 @@
       <c r="P285"/>
       <c r="Q285"/>
       <c r="R285"/>
-      <c r="S285" t="s">
-        <v>320</v>
-      </c>
+      <c r="S285"/>
       <c r="T285"/>
       <c r="U285"/>
       <c r="V285"/>
@@ -14759,11 +14758,11 @@
       <c r="G286"/>
       <c r="H286"/>
       <c r="I286"/>
-      <c r="J286" t="s">
+      <c r="J286"/>
+      <c r="K286"/>
+      <c r="L286" t="s">
         <v>321</v>
       </c>
-      <c r="K286"/>
-      <c r="L286"/>
       <c r="M286"/>
       <c r="N286"/>
       <c r="O286"/>
@@ -14836,12 +14835,12 @@
       <c r="F288"/>
       <c r="G288"/>
       <c r="H288"/>
-      <c r="I288"/>
+      <c r="I288" t="s">
+        <v>323</v>
+      </c>
       <c r="J288"/>
       <c r="K288"/>
-      <c r="L288" t="s">
-        <v>323</v>
-      </c>
+      <c r="L288"/>
       <c r="M288"/>
       <c r="N288"/>
       <c r="O288"/>
@@ -14861,13 +14860,13 @@
         <v>324</v>
       </c>
       <c r="B289" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C289" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D289" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E289" t="n">
         <v>5</v>
@@ -14875,14 +14874,14 @@
       <c r="F289"/>
       <c r="G289"/>
       <c r="H289"/>
-      <c r="I289" t="s">
-        <v>324</v>
-      </c>
+      <c r="I289"/>
       <c r="J289"/>
       <c r="K289"/>
       <c r="L289"/>
       <c r="M289"/>
-      <c r="N289"/>
+      <c r="N289" t="s">
+        <v>324</v>
+      </c>
       <c r="O289"/>
       <c r="P289"/>
       <c r="Q289"/>
@@ -14939,13 +14938,13 @@
         <v>326</v>
       </c>
       <c r="B291" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C291" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D291" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="E291" t="n">
         <v>5</v>
@@ -14957,10 +14956,10 @@
       <c r="J291"/>
       <c r="K291"/>
       <c r="L291"/>
-      <c r="M291"/>
-      <c r="N291" t="s">
+      <c r="M291" t="s">
         <v>326</v>
       </c>
+      <c r="N291"/>
       <c r="O291"/>
       <c r="P291"/>
       <c r="Q291"/>
@@ -14995,10 +14994,10 @@
       <c r="I292"/>
       <c r="J292"/>
       <c r="K292"/>
-      <c r="L292"/>
-      <c r="M292" t="s">
+      <c r="L292" t="s">
         <v>327</v>
       </c>
+      <c r="M292"/>
       <c r="N292"/>
       <c r="O292"/>
       <c r="P292"/>
@@ -15017,13 +15016,13 @@
         <v>328</v>
       </c>
       <c r="B293" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="C293" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="D293" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="E293" t="n">
         <v>5</v>
@@ -15034,16 +15033,16 @@
       <c r="I293"/>
       <c r="J293"/>
       <c r="K293"/>
-      <c r="L293" t="s">
-        <v>328</v>
-      </c>
+      <c r="L293"/>
       <c r="M293"/>
       <c r="N293"/>
       <c r="O293"/>
       <c r="P293"/>
       <c r="Q293"/>
       <c r="R293"/>
-      <c r="S293"/>
+      <c r="S293" t="s">
+        <v>328</v>
+      </c>
       <c r="T293"/>
       <c r="U293"/>
       <c r="V293"/>
@@ -15056,13 +15055,13 @@
         <v>329</v>
       </c>
       <c r="B294" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="C294" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="D294" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="E294" t="n">
         <v>5</v>
@@ -15075,14 +15074,14 @@
       <c r="K294"/>
       <c r="L294"/>
       <c r="M294"/>
-      <c r="N294"/>
+      <c r="N294" t="s">
+        <v>329</v>
+      </c>
       <c r="O294"/>
       <c r="P294"/>
       <c r="Q294"/>
       <c r="R294"/>
-      <c r="S294" t="s">
-        <v>329</v>
-      </c>
+      <c r="S294"/>
       <c r="T294"/>
       <c r="U294"/>
       <c r="V294"/>
@@ -15173,13 +15172,13 @@
         <v>332</v>
       </c>
       <c r="B297" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C297" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D297" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="E297" t="n">
         <v>5</v>
@@ -15192,14 +15191,14 @@
       <c r="K297"/>
       <c r="L297"/>
       <c r="M297"/>
-      <c r="N297" t="s">
-        <v>332</v>
-      </c>
+      <c r="N297"/>
       <c r="O297"/>
       <c r="P297"/>
       <c r="Q297"/>
       <c r="R297"/>
-      <c r="S297"/>
+      <c r="S297" t="s">
+        <v>332</v>
+      </c>
       <c r="T297"/>
       <c r="U297"/>
       <c r="V297"/>
@@ -15212,20 +15211,22 @@
         <v>333</v>
       </c>
       <c r="B298" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C298" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="D298" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="E298" t="n">
         <v>5</v>
       </c>
       <c r="F298"/>
       <c r="G298"/>
-      <c r="H298"/>
+      <c r="H298" t="s">
+        <v>333</v>
+      </c>
       <c r="I298"/>
       <c r="J298"/>
       <c r="K298"/>
@@ -15236,9 +15237,7 @@
       <c r="P298"/>
       <c r="Q298"/>
       <c r="R298"/>
-      <c r="S298" t="s">
-        <v>333</v>
-      </c>
+      <c r="S298"/>
       <c r="T298"/>
       <c r="U298"/>
       <c r="V298"/>
@@ -15264,13 +15263,13 @@
       </c>
       <c r="F299"/>
       <c r="G299"/>
-      <c r="H299" t="s">
-        <v>334</v>
-      </c>
+      <c r="H299"/>
       <c r="I299"/>
       <c r="J299"/>
       <c r="K299"/>
-      <c r="L299"/>
+      <c r="L299" t="s">
+        <v>334</v>
+      </c>
       <c r="M299"/>
       <c r="N299"/>
       <c r="O299"/>
@@ -15290,13 +15289,13 @@
         <v>335</v>
       </c>
       <c r="B300" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C300" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D300" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E300" t="n">
         <v>5</v>
@@ -15307,14 +15306,14 @@
       <c r="I300"/>
       <c r="J300"/>
       <c r="K300"/>
-      <c r="L300" t="s">
-        <v>335</v>
-      </c>
+      <c r="L300"/>
       <c r="M300"/>
       <c r="N300"/>
       <c r="O300"/>
       <c r="P300"/>
-      <c r="Q300"/>
+      <c r="Q300" t="s">
+        <v>335</v>
+      </c>
       <c r="R300"/>
       <c r="S300"/>
       <c r="T300"/>
@@ -15329,13 +15328,13 @@
         <v>336</v>
       </c>
       <c r="B301" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C301" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D301" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E301" t="n">
         <v>5</v>
@@ -15383,16 +15382,16 @@
       <c r="G302"/>
       <c r="H302"/>
       <c r="I302"/>
-      <c r="J302"/>
+      <c r="J302" t="s">
+        <v>337</v>
+      </c>
       <c r="K302"/>
       <c r="L302"/>
       <c r="M302"/>
       <c r="N302"/>
       <c r="O302"/>
       <c r="P302"/>
-      <c r="Q302" t="s">
-        <v>337</v>
-      </c>
+      <c r="Q302"/>
       <c r="R302"/>
       <c r="S302"/>
       <c r="T302"/>
@@ -15422,11 +15421,11 @@
       <c r="G303"/>
       <c r="H303"/>
       <c r="I303"/>
-      <c r="J303" t="s">
+      <c r="J303"/>
+      <c r="K303"/>
+      <c r="L303" t="s">
         <v>338</v>
       </c>
-      <c r="K303"/>
-      <c r="L303"/>
       <c r="M303"/>
       <c r="N303"/>
       <c r="O303"/>
@@ -15502,9 +15501,7 @@
       <c r="I305"/>
       <c r="J305"/>
       <c r="K305"/>
-      <c r="L305" t="s">
-        <v>340</v>
-      </c>
+      <c r="L305"/>
       <c r="M305"/>
       <c r="N305"/>
       <c r="O305"/>
@@ -15515,7 +15512,9 @@
       <c r="T305"/>
       <c r="U305"/>
       <c r="V305"/>
-      <c r="W305"/>
+      <c r="W305" t="s">
+        <v>340</v>
+      </c>
       <c r="X305"/>
       <c r="Y305"/>
     </row>
@@ -15524,20 +15523,22 @@
         <v>341</v>
       </c>
       <c r="B306" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C306" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D306" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E306" t="n">
         <v>5</v>
       </c>
       <c r="F306"/>
       <c r="G306"/>
-      <c r="H306"/>
+      <c r="H306" t="s">
+        <v>341</v>
+      </c>
       <c r="I306"/>
       <c r="J306"/>
       <c r="K306"/>
@@ -15552,9 +15553,7 @@
       <c r="T306"/>
       <c r="U306"/>
       <c r="V306"/>
-      <c r="W306" t="s">
-        <v>341</v>
-      </c>
+      <c r="W306"/>
       <c r="X306"/>
       <c r="Y306"/>
     </row>
@@ -15576,9 +15575,7 @@
       </c>
       <c r="F307"/>
       <c r="G307"/>
-      <c r="H307" t="s">
-        <v>342</v>
-      </c>
+      <c r="H307"/>
       <c r="I307"/>
       <c r="J307"/>
       <c r="K307"/>
@@ -15588,7 +15585,9 @@
       <c r="O307"/>
       <c r="P307"/>
       <c r="Q307"/>
-      <c r="R307"/>
+      <c r="R307" t="s">
+        <v>342</v>
+      </c>
       <c r="S307"/>
       <c r="T307"/>
       <c r="U307"/>
@@ -15602,13 +15601,13 @@
         <v>343</v>
       </c>
       <c r="B308" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="C308" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D308" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="E308" t="n">
         <v>5</v>
@@ -15619,15 +15618,15 @@
       <c r="I308"/>
       <c r="J308"/>
       <c r="K308"/>
-      <c r="L308"/>
+      <c r="L308" t="s">
+        <v>343</v>
+      </c>
       <c r="M308"/>
       <c r="N308"/>
       <c r="O308"/>
       <c r="P308"/>
       <c r="Q308"/>
-      <c r="R308" t="s">
-        <v>343</v>
-      </c>
+      <c r="R308"/>
       <c r="S308"/>
       <c r="T308"/>
       <c r="U308"/>
@@ -15641,13 +15640,13 @@
         <v>344</v>
       </c>
       <c r="B309" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="C309" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="D309" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="E309" t="n">
         <v>5</v>
@@ -15658,11 +15657,11 @@
       <c r="I309"/>
       <c r="J309"/>
       <c r="K309"/>
-      <c r="L309" t="s">
+      <c r="L309"/>
+      <c r="M309"/>
+      <c r="N309" t="s">
         <v>344</v>
       </c>
-      <c r="M309"/>
-      <c r="N309"/>
       <c r="O309"/>
       <c r="P309"/>
       <c r="Q309"/>
@@ -15699,10 +15698,10 @@
       <c r="K310"/>
       <c r="L310"/>
       <c r="M310"/>
-      <c r="N310" t="s">
+      <c r="N310"/>
+      <c r="O310" t="s">
         <v>345</v>
       </c>
-      <c r="O310"/>
       <c r="P310"/>
       <c r="Q310"/>
       <c r="R310"/>
@@ -15719,13 +15718,13 @@
         <v>346</v>
       </c>
       <c r="B311" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C311" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D311" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E311" t="n">
         <v>5</v>
@@ -15736,12 +15735,12 @@
       <c r="I311"/>
       <c r="J311"/>
       <c r="K311"/>
-      <c r="L311"/>
+      <c r="L311" t="s">
+        <v>346</v>
+      </c>
       <c r="M311"/>
       <c r="N311"/>
-      <c r="O311" t="s">
-        <v>346</v>
-      </c>
+      <c r="O311"/>
       <c r="P311"/>
       <c r="Q311"/>
       <c r="R311"/>
@@ -15758,13 +15757,13 @@
         <v>347</v>
       </c>
       <c r="B312" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C312" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D312" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="E312" t="n">
         <v>5</v>
@@ -15772,12 +15771,12 @@
       <c r="F312"/>
       <c r="G312"/>
       <c r="H312"/>
-      <c r="I312"/>
+      <c r="I312" t="s">
+        <v>347</v>
+      </c>
       <c r="J312"/>
       <c r="K312"/>
-      <c r="L312" t="s">
-        <v>347</v>
-      </c>
+      <c r="L312"/>
       <c r="M312"/>
       <c r="N312"/>
       <c r="O312"/>
@@ -15811,10 +15810,10 @@
       <c r="F313"/>
       <c r="G313"/>
       <c r="H313"/>
-      <c r="I313" t="s">
+      <c r="I313"/>
+      <c r="J313" t="s">
         <v>348</v>
       </c>
-      <c r="J313"/>
       <c r="K313"/>
       <c r="L313"/>
       <c r="M313"/>
@@ -15849,11 +15848,11 @@
       </c>
       <c r="F314"/>
       <c r="G314"/>
-      <c r="H314"/>
+      <c r="H314" t="s">
+        <v>349</v>
+      </c>
       <c r="I314"/>
-      <c r="J314" t="s">
-        <v>349</v>
-      </c>
+      <c r="J314"/>
       <c r="K314"/>
       <c r="L314"/>
       <c r="M314"/>
@@ -15875,13 +15874,13 @@
         <v>350</v>
       </c>
       <c r="B315" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C315" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D315" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E315" t="n">
         <v>5</v>
@@ -15927,13 +15926,13 @@
       </c>
       <c r="F316"/>
       <c r="G316"/>
-      <c r="H316" t="s">
-        <v>351</v>
-      </c>
+      <c r="H316"/>
       <c r="I316"/>
       <c r="J316"/>
       <c r="K316"/>
-      <c r="L316"/>
+      <c r="L316" t="s">
+        <v>351</v>
+      </c>
       <c r="M316"/>
       <c r="N316"/>
       <c r="O316"/>
@@ -15992,13 +15991,13 @@
         <v>353</v>
       </c>
       <c r="B318" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C318" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D318" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E318" t="n">
         <v>5</v>
@@ -16006,12 +16005,12 @@
       <c r="F318"/>
       <c r="G318"/>
       <c r="H318"/>
-      <c r="I318"/>
+      <c r="I318" t="s">
+        <v>353</v>
+      </c>
       <c r="J318"/>
       <c r="K318"/>
-      <c r="L318" t="s">
-        <v>353</v>
-      </c>
+      <c r="L318"/>
       <c r="M318"/>
       <c r="N318"/>
       <c r="O318"/>
@@ -16045,10 +16044,10 @@
       <c r="F319"/>
       <c r="G319"/>
       <c r="H319"/>
-      <c r="I319" t="s">
+      <c r="I319"/>
+      <c r="J319" t="s">
         <v>354</v>
       </c>
-      <c r="J319"/>
       <c r="K319"/>
       <c r="L319"/>
       <c r="M319"/>
@@ -16083,11 +16082,11 @@
       </c>
       <c r="F320"/>
       <c r="G320"/>
-      <c r="H320"/>
+      <c r="H320" t="s">
+        <v>355</v>
+      </c>
       <c r="I320"/>
-      <c r="J320" t="s">
-        <v>355</v>
-      </c>
+      <c r="J320"/>
       <c r="K320"/>
       <c r="L320"/>
       <c r="M320"/>
@@ -16109,22 +16108,20 @@
         <v>356</v>
       </c>
       <c r="B321" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C321" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D321" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E321" t="n">
         <v>5</v>
       </c>
       <c r="F321"/>
       <c r="G321"/>
-      <c r="H321" t="s">
-        <v>356</v>
-      </c>
+      <c r="H321"/>
       <c r="I321"/>
       <c r="J321"/>
       <c r="K321"/>
@@ -16133,7 +16130,9 @@
       <c r="N321"/>
       <c r="O321"/>
       <c r="P321"/>
-      <c r="Q321"/>
+      <c r="Q321" t="s">
+        <v>356</v>
+      </c>
       <c r="R321"/>
       <c r="S321"/>
       <c r="T321"/>
@@ -16148,13 +16147,13 @@
         <v>357</v>
       </c>
       <c r="B322" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C322" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D322" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E322" t="n">
         <v>5</v>
@@ -16170,11 +16169,11 @@
       <c r="N322"/>
       <c r="O322"/>
       <c r="P322"/>
-      <c r="Q322" t="s">
+      <c r="Q322"/>
+      <c r="R322"/>
+      <c r="S322" t="s">
         <v>357</v>
       </c>
-      <c r="R322"/>
-      <c r="S322"/>
       <c r="T322"/>
       <c r="U322"/>
       <c r="V322"/>
@@ -16209,11 +16208,11 @@
       <c r="N323"/>
       <c r="O323"/>
       <c r="P323"/>
-      <c r="Q323"/>
+      <c r="Q323" t="s">
+        <v>358</v>
+      </c>
       <c r="R323"/>
-      <c r="S323" t="s">
-        <v>358</v>
-      </c>
+      <c r="S323"/>
       <c r="T323"/>
       <c r="U323"/>
       <c r="V323"/>
@@ -16265,13 +16264,13 @@
         <v>360</v>
       </c>
       <c r="B325" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C325" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D325" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E325" t="n">
         <v>5</v>
@@ -16287,11 +16286,11 @@
       <c r="N325"/>
       <c r="O325"/>
       <c r="P325"/>
-      <c r="Q325" t="s">
+      <c r="Q325"/>
+      <c r="R325"/>
+      <c r="S325" t="s">
         <v>360</v>
       </c>
-      <c r="R325"/>
-      <c r="S325"/>
       <c r="T325"/>
       <c r="U325"/>
       <c r="V325"/>
@@ -16319,7 +16318,9 @@
       <c r="G326"/>
       <c r="H326"/>
       <c r="I326"/>
-      <c r="J326"/>
+      <c r="J326" t="s">
+        <v>361</v>
+      </c>
       <c r="K326"/>
       <c r="L326"/>
       <c r="M326"/>
@@ -16328,9 +16329,7 @@
       <c r="P326"/>
       <c r="Q326"/>
       <c r="R326"/>
-      <c r="S326" t="s">
-        <v>361</v>
-      </c>
+      <c r="S326"/>
       <c r="T326"/>
       <c r="U326"/>
       <c r="V326"/>
@@ -16343,13 +16342,13 @@
         <v>362</v>
       </c>
       <c r="B327" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C327" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D327" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E327" t="n">
         <v>5</v>
@@ -16358,14 +16357,14 @@
       <c r="G327"/>
       <c r="H327"/>
       <c r="I327"/>
-      <c r="J327" t="s">
-        <v>362</v>
-      </c>
+      <c r="J327"/>
       <c r="K327"/>
       <c r="L327"/>
       <c r="M327"/>
       <c r="N327"/>
-      <c r="O327"/>
+      <c r="O327" t="s">
+        <v>362</v>
+      </c>
       <c r="P327"/>
       <c r="Q327"/>
       <c r="R327"/>
@@ -16382,13 +16381,13 @@
         <v>363</v>
       </c>
       <c r="B328" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C328" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D328" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E328" t="n">
         <v>5</v>
@@ -16397,14 +16396,14 @@
       <c r="G328"/>
       <c r="H328"/>
       <c r="I328"/>
-      <c r="J328"/>
+      <c r="J328" t="s">
+        <v>363</v>
+      </c>
       <c r="K328"/>
       <c r="L328"/>
       <c r="M328"/>
       <c r="N328"/>
-      <c r="O328" t="s">
-        <v>363</v>
-      </c>
+      <c r="O328"/>
       <c r="P328"/>
       <c r="Q328"/>
       <c r="R328"/>
@@ -16436,9 +16435,7 @@
       <c r="G329"/>
       <c r="H329"/>
       <c r="I329"/>
-      <c r="J329" t="s">
-        <v>364</v>
-      </c>
+      <c r="J329"/>
       <c r="K329"/>
       <c r="L329"/>
       <c r="M329"/>
@@ -16446,7 +16443,9 @@
       <c r="O329"/>
       <c r="P329"/>
       <c r="Q329"/>
-      <c r="R329"/>
+      <c r="R329" t="s">
+        <v>364</v>
+      </c>
       <c r="S329"/>
       <c r="T329"/>
       <c r="U329"/>
@@ -16474,7 +16473,9 @@
       <c r="F330"/>
       <c r="G330"/>
       <c r="H330"/>
-      <c r="I330"/>
+      <c r="I330" t="s">
+        <v>365</v>
+      </c>
       <c r="J330"/>
       <c r="K330"/>
       <c r="L330"/>
@@ -16483,9 +16484,7 @@
       <c r="O330"/>
       <c r="P330"/>
       <c r="Q330"/>
-      <c r="R330" t="s">
-        <v>365</v>
-      </c>
+      <c r="R330"/>
       <c r="S330"/>
       <c r="T330"/>
       <c r="U330"/>
@@ -16512,10 +16511,10 @@
       </c>
       <c r="F331"/>
       <c r="G331"/>
-      <c r="H331"/>
-      <c r="I331" t="s">
+      <c r="H331" t="s">
         <v>366</v>
       </c>
+      <c r="I331"/>
       <c r="J331"/>
       <c r="K331"/>
       <c r="L331"/>
@@ -16707,13 +16706,13 @@
       </c>
       <c r="F336"/>
       <c r="G336"/>
-      <c r="H336" t="s">
-        <v>371</v>
-      </c>
+      <c r="H336"/>
       <c r="I336"/>
       <c r="J336"/>
       <c r="K336"/>
-      <c r="L336"/>
+      <c r="L336" t="s">
+        <v>371</v>
+      </c>
       <c r="M336"/>
       <c r="N336"/>
       <c r="O336"/>
@@ -16733,13 +16732,13 @@
         <v>372</v>
       </c>
       <c r="B337" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C337" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D337" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E337" t="n">
         <v>5</v>
@@ -16750,11 +16749,11 @@
       <c r="I337"/>
       <c r="J337"/>
       <c r="K337"/>
-      <c r="L337" t="s">
+      <c r="L337"/>
+      <c r="M337"/>
+      <c r="N337" t="s">
         <v>372</v>
       </c>
-      <c r="M337"/>
-      <c r="N337"/>
       <c r="O337"/>
       <c r="P337"/>
       <c r="Q337"/>
@@ -16772,13 +16771,13 @@
         <v>373</v>
       </c>
       <c r="B338" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C338" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D338" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E338" t="n">
         <v>5</v>
@@ -16791,13 +16790,13 @@
       <c r="K338"/>
       <c r="L338"/>
       <c r="M338"/>
-      <c r="N338" t="s">
-        <v>373</v>
-      </c>
+      <c r="N338"/>
       <c r="O338"/>
       <c r="P338"/>
       <c r="Q338"/>
-      <c r="R338"/>
+      <c r="R338" t="s">
+        <v>373</v>
+      </c>
       <c r="S338"/>
       <c r="T338"/>
       <c r="U338"/>
@@ -16824,7 +16823,9 @@
       </c>
       <c r="F339"/>
       <c r="G339"/>
-      <c r="H339"/>
+      <c r="H339" t="s">
+        <v>374</v>
+      </c>
       <c r="I339"/>
       <c r="J339"/>
       <c r="K339"/>
@@ -16834,9 +16835,7 @@
       <c r="O339"/>
       <c r="P339"/>
       <c r="Q339"/>
-      <c r="R339" t="s">
-        <v>374</v>
-      </c>
+      <c r="R339"/>
       <c r="S339"/>
       <c r="T339"/>
       <c r="U339"/>
@@ -16902,10 +16901,10 @@
       </c>
       <c r="F341"/>
       <c r="G341"/>
-      <c r="H341" t="s">
+      <c r="H341"/>
+      <c r="I341" t="s">
         <v>376</v>
       </c>
-      <c r="I341"/>
       <c r="J341"/>
       <c r="K341"/>
       <c r="L341"/>
@@ -16942,12 +16941,12 @@
       <c r="F342"/>
       <c r="G342"/>
       <c r="H342"/>
-      <c r="I342" t="s">
-        <v>377</v>
-      </c>
+      <c r="I342"/>
       <c r="J342"/>
       <c r="K342"/>
-      <c r="L342"/>
+      <c r="L342" t="s">
+        <v>377</v>
+      </c>
       <c r="M342"/>
       <c r="N342"/>
       <c r="O342"/>
@@ -16984,15 +16983,15 @@
       <c r="I343"/>
       <c r="J343"/>
       <c r="K343"/>
-      <c r="L343" t="s">
-        <v>378</v>
-      </c>
+      <c r="L343"/>
       <c r="M343"/>
       <c r="N343"/>
       <c r="O343"/>
       <c r="P343"/>
       <c r="Q343"/>
-      <c r="R343"/>
+      <c r="R343" t="s">
+        <v>378</v>
+      </c>
       <c r="S343"/>
       <c r="T343"/>
       <c r="U343"/>
@@ -17025,13 +17024,13 @@
       <c r="K344"/>
       <c r="L344"/>
       <c r="M344"/>
-      <c r="N344"/>
+      <c r="N344" t="s">
+        <v>379</v>
+      </c>
       <c r="O344"/>
       <c r="P344"/>
       <c r="Q344"/>
-      <c r="R344" t="s">
-        <v>379</v>
-      </c>
+      <c r="R344"/>
       <c r="S344"/>
       <c r="T344"/>
       <c r="U344"/>
@@ -17103,14 +17102,14 @@
       <c r="K346"/>
       <c r="L346"/>
       <c r="M346"/>
-      <c r="N346" t="s">
-        <v>381</v>
-      </c>
+      <c r="N346"/>
       <c r="O346"/>
       <c r="P346"/>
       <c r="Q346"/>
       <c r="R346"/>
-      <c r="S346"/>
+      <c r="S346" t="s">
+        <v>381</v>
+      </c>
       <c r="T346"/>
       <c r="U346"/>
       <c r="V346"/>
@@ -17179,16 +17178,16 @@
       <c r="I348"/>
       <c r="J348"/>
       <c r="K348"/>
-      <c r="L348"/>
+      <c r="L348" t="s">
+        <v>383</v>
+      </c>
       <c r="M348"/>
       <c r="N348"/>
       <c r="O348"/>
       <c r="P348"/>
       <c r="Q348"/>
       <c r="R348"/>
-      <c r="S348" t="s">
-        <v>383</v>
-      </c>
+      <c r="S348"/>
       <c r="T348"/>
       <c r="U348"/>
       <c r="V348"/>
@@ -17216,11 +17215,11 @@
       <c r="G349"/>
       <c r="H349"/>
       <c r="I349"/>
-      <c r="J349"/>
+      <c r="J349" t="s">
+        <v>384</v>
+      </c>
       <c r="K349"/>
-      <c r="L349" t="s">
-        <v>384</v>
-      </c>
+      <c r="L349"/>
       <c r="M349"/>
       <c r="N349"/>
       <c r="O349"/>
@@ -17255,11 +17254,11 @@
       <c r="G350"/>
       <c r="H350"/>
       <c r="I350"/>
-      <c r="J350" t="s">
+      <c r="J350"/>
+      <c r="K350"/>
+      <c r="L350" t="s">
         <v>385</v>
       </c>
-      <c r="K350"/>
-      <c r="L350"/>
       <c r="M350"/>
       <c r="N350"/>
       <c r="O350"/>
@@ -17294,11 +17293,11 @@
       <c r="G351"/>
       <c r="H351"/>
       <c r="I351"/>
-      <c r="J351"/>
+      <c r="J351" t="s">
+        <v>386</v>
+      </c>
       <c r="K351"/>
-      <c r="L351" t="s">
-        <v>386</v>
-      </c>
+      <c r="L351"/>
       <c r="M351"/>
       <c r="N351"/>
       <c r="O351"/>
@@ -17318,13 +17317,13 @@
         <v>387</v>
       </c>
       <c r="B352" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C352" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D352" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E352" t="n">
         <v>5</v>
@@ -17333,13 +17332,13 @@
       <c r="G352"/>
       <c r="H352"/>
       <c r="I352"/>
-      <c r="J352" t="s">
-        <v>387</v>
-      </c>
+      <c r="J352"/>
       <c r="K352"/>
       <c r="L352"/>
       <c r="M352"/>
-      <c r="N352"/>
+      <c r="N352" t="s">
+        <v>387</v>
+      </c>
       <c r="O352"/>
       <c r="P352"/>
       <c r="Q352"/>
@@ -17376,12 +17375,12 @@
       <c r="K353"/>
       <c r="L353"/>
       <c r="M353"/>
-      <c r="N353" t="s">
-        <v>388</v>
-      </c>
+      <c r="N353"/>
       <c r="O353"/>
       <c r="P353"/>
-      <c r="Q353"/>
+      <c r="Q353" t="s">
+        <v>388</v>
+      </c>
       <c r="R353"/>
       <c r="S353"/>
       <c r="T353"/>
@@ -17396,13 +17395,13 @@
         <v>389</v>
       </c>
       <c r="B354" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C354" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D354" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E354" t="n">
         <v>5</v>
@@ -17415,12 +17414,12 @@
       <c r="K354"/>
       <c r="L354"/>
       <c r="M354"/>
-      <c r="N354"/>
+      <c r="N354" t="s">
+        <v>389</v>
+      </c>
       <c r="O354"/>
       <c r="P354"/>
-      <c r="Q354" t="s">
-        <v>389</v>
-      </c>
+      <c r="Q354"/>
       <c r="R354"/>
       <c r="S354"/>
       <c r="T354"/>
@@ -17450,13 +17449,13 @@
       <c r="G355"/>
       <c r="H355"/>
       <c r="I355"/>
-      <c r="J355"/>
+      <c r="J355" t="s">
+        <v>390</v>
+      </c>
       <c r="K355"/>
       <c r="L355"/>
       <c r="M355"/>
-      <c r="N355" t="s">
-        <v>390</v>
-      </c>
+      <c r="N355"/>
       <c r="O355"/>
       <c r="P355"/>
       <c r="Q355"/>
@@ -17474,13 +17473,13 @@
         <v>391</v>
       </c>
       <c r="B356" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="C356" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="D356" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="E356" t="n">
         <v>5</v>
@@ -17489,9 +17488,7 @@
       <c r="G356"/>
       <c r="H356"/>
       <c r="I356"/>
-      <c r="J356" t="s">
-        <v>391</v>
-      </c>
+      <c r="J356"/>
       <c r="K356"/>
       <c r="L356"/>
       <c r="M356"/>
@@ -17500,7 +17497,9 @@
       <c r="P356"/>
       <c r="Q356"/>
       <c r="R356"/>
-      <c r="S356"/>
+      <c r="S356" t="s">
+        <v>391</v>
+      </c>
       <c r="T356"/>
       <c r="U356"/>
       <c r="V356"/>
@@ -17513,13 +17512,13 @@
         <v>392</v>
       </c>
       <c r="B357" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="C357" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="D357" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="E357" t="n">
         <v>5</v>
@@ -17552,13 +17551,13 @@
         <v>393</v>
       </c>
       <c r="B358" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C358" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D358" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E358" t="n">
         <v>5</v>
@@ -17569,16 +17568,16 @@
       <c r="I358"/>
       <c r="J358"/>
       <c r="K358"/>
-      <c r="L358"/>
+      <c r="L358" t="s">
+        <v>393</v>
+      </c>
       <c r="M358"/>
       <c r="N358"/>
       <c r="O358"/>
       <c r="P358"/>
       <c r="Q358"/>
       <c r="R358"/>
-      <c r="S358" t="s">
-        <v>393</v>
-      </c>
+      <c r="S358"/>
       <c r="T358"/>
       <c r="U358"/>
       <c r="V358"/>
@@ -17669,13 +17668,13 @@
         <v>396</v>
       </c>
       <c r="B361" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C361" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D361" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E361" t="n">
         <v>5</v>
@@ -17686,9 +17685,7 @@
       <c r="I361"/>
       <c r="J361"/>
       <c r="K361"/>
-      <c r="L361" t="s">
-        <v>396</v>
-      </c>
+      <c r="L361"/>
       <c r="M361"/>
       <c r="N361"/>
       <c r="O361"/>
@@ -17696,7 +17693,9 @@
       <c r="Q361"/>
       <c r="R361"/>
       <c r="S361"/>
-      <c r="T361"/>
+      <c r="T361" t="s">
+        <v>396</v>
+      </c>
       <c r="U361"/>
       <c r="V361"/>
       <c r="W361"/>
@@ -17729,13 +17728,13 @@
       <c r="M362"/>
       <c r="N362"/>
       <c r="O362"/>
-      <c r="P362"/>
+      <c r="P362" t="s">
+        <v>397</v>
+      </c>
       <c r="Q362"/>
       <c r="R362"/>
       <c r="S362"/>
-      <c r="T362" t="s">
-        <v>397</v>
-      </c>
+      <c r="T362"/>
       <c r="U362"/>
       <c r="V362"/>
       <c r="W362"/>
@@ -17747,13 +17746,13 @@
         <v>398</v>
       </c>
       <c r="B363" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="C363" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D363" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="E363" t="n">
         <v>5</v>
@@ -17768,11 +17767,11 @@
       <c r="M363"/>
       <c r="N363"/>
       <c r="O363"/>
-      <c r="P363" t="s">
+      <c r="P363"/>
+      <c r="Q363"/>
+      <c r="R363" t="s">
         <v>398</v>
       </c>
-      <c r="Q363"/>
-      <c r="R363"/>
       <c r="S363"/>
       <c r="T363"/>
       <c r="U363"/>
@@ -17786,13 +17785,13 @@
         <v>399</v>
       </c>
       <c r="B364" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="C364" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="D364" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="E364" t="n">
         <v>5</v>
@@ -17809,12 +17808,12 @@
       <c r="O364"/>
       <c r="P364"/>
       <c r="Q364"/>
-      <c r="R364" t="s">
-        <v>399</v>
-      </c>
+      <c r="R364"/>
       <c r="S364"/>
       <c r="T364"/>
-      <c r="U364"/>
+      <c r="U364" t="s">
+        <v>399</v>
+      </c>
       <c r="V364"/>
       <c r="W364"/>
       <c r="X364"/>
@@ -17846,14 +17845,14 @@
       <c r="M365"/>
       <c r="N365"/>
       <c r="O365"/>
-      <c r="P365"/>
+      <c r="P365" t="s">
+        <v>400</v>
+      </c>
       <c r="Q365"/>
       <c r="R365"/>
       <c r="S365"/>
       <c r="T365"/>
-      <c r="U365" t="s">
-        <v>400</v>
-      </c>
+      <c r="U365"/>
       <c r="V365"/>
       <c r="W365"/>
       <c r="X365"/>
@@ -17883,11 +17882,11 @@
       <c r="K366"/>
       <c r="L366"/>
       <c r="M366"/>
-      <c r="N366"/>
+      <c r="N366" t="s">
+        <v>401</v>
+      </c>
       <c r="O366"/>
-      <c r="P366" t="s">
-        <v>401</v>
-      </c>
+      <c r="P366"/>
       <c r="Q366"/>
       <c r="R366"/>
       <c r="S366"/>
@@ -17922,14 +17921,14 @@
       <c r="K367"/>
       <c r="L367"/>
       <c r="M367"/>
-      <c r="N367" t="s">
-        <v>402</v>
-      </c>
+      <c r="N367"/>
       <c r="O367"/>
       <c r="P367"/>
       <c r="Q367"/>
       <c r="R367"/>
-      <c r="S367"/>
+      <c r="S367" t="s">
+        <v>402</v>
+      </c>
       <c r="T367"/>
       <c r="U367"/>
       <c r="V367"/>
@@ -17965,10 +17964,10 @@
       <c r="O368"/>
       <c r="P368"/>
       <c r="Q368"/>
-      <c r="R368"/>
-      <c r="S368" t="s">
+      <c r="R368" t="s">
         <v>403</v>
       </c>
+      <c r="S368"/>
       <c r="T368"/>
       <c r="U368"/>
       <c r="V368"/>
@@ -18001,12 +18000,12 @@
       <c r="L369"/>
       <c r="M369"/>
       <c r="N369"/>
-      <c r="O369"/>
+      <c r="O369" t="s">
+        <v>404</v>
+      </c>
       <c r="P369"/>
       <c r="Q369"/>
-      <c r="R369" t="s">
-        <v>404</v>
-      </c>
+      <c r="R369"/>
       <c r="S369"/>
       <c r="T369"/>
       <c r="U369"/>
@@ -18035,14 +18034,14 @@
       <c r="G370"/>
       <c r="H370"/>
       <c r="I370"/>
-      <c r="J370"/>
+      <c r="J370" t="s">
+        <v>405</v>
+      </c>
       <c r="K370"/>
       <c r="L370"/>
       <c r="M370"/>
       <c r="N370"/>
-      <c r="O370" t="s">
-        <v>405</v>
-      </c>
+      <c r="O370"/>
       <c r="P370"/>
       <c r="Q370"/>
       <c r="R370"/>
@@ -18074,11 +18073,11 @@
       <c r="G371"/>
       <c r="H371"/>
       <c r="I371"/>
-      <c r="J371" t="s">
+      <c r="J371"/>
+      <c r="K371"/>
+      <c r="L371" t="s">
         <v>406</v>
       </c>
-      <c r="K371"/>
-      <c r="L371"/>
       <c r="M371"/>
       <c r="N371"/>
       <c r="O371"/>
@@ -18115,11 +18114,11 @@
       <c r="I372"/>
       <c r="J372"/>
       <c r="K372"/>
-      <c r="L372" t="s">
+      <c r="L372"/>
+      <c r="M372"/>
+      <c r="N372" t="s">
         <v>407</v>
       </c>
-      <c r="M372"/>
-      <c r="N372"/>
       <c r="O372"/>
       <c r="P372"/>
       <c r="Q372"/>
@@ -18150,15 +18149,15 @@
       </c>
       <c r="F373"/>
       <c r="G373"/>
-      <c r="H373"/>
+      <c r="H373" t="s">
+        <v>408</v>
+      </c>
       <c r="I373"/>
       <c r="J373"/>
       <c r="K373"/>
       <c r="L373"/>
       <c r="M373"/>
-      <c r="N373" t="s">
-        <v>408</v>
-      </c>
+      <c r="N373"/>
       <c r="O373"/>
       <c r="P373"/>
       <c r="Q373"/>
@@ -18228,9 +18227,7 @@
       </c>
       <c r="F375"/>
       <c r="G375"/>
-      <c r="H375" t="s">
-        <v>410</v>
-      </c>
+      <c r="H375"/>
       <c r="I375"/>
       <c r="J375"/>
       <c r="K375"/>
@@ -18240,7 +18237,9 @@
       <c r="O375"/>
       <c r="P375"/>
       <c r="Q375"/>
-      <c r="R375"/>
+      <c r="R375" t="s">
+        <v>410</v>
+      </c>
       <c r="S375"/>
       <c r="T375"/>
       <c r="U375"/>
@@ -18273,13 +18272,13 @@
       <c r="K376"/>
       <c r="L376"/>
       <c r="M376"/>
-      <c r="N376"/>
+      <c r="N376" t="s">
+        <v>411</v>
+      </c>
       <c r="O376"/>
       <c r="P376"/>
       <c r="Q376"/>
-      <c r="R376" t="s">
-        <v>411</v>
-      </c>
+      <c r="R376"/>
       <c r="S376"/>
       <c r="T376"/>
       <c r="U376"/>
@@ -18293,13 +18292,13 @@
         <v>412</v>
       </c>
       <c r="B377" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="C377" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="D377" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="E377" t="n">
         <v>5</v>
@@ -18312,14 +18311,14 @@
       <c r="K377"/>
       <c r="L377"/>
       <c r="M377"/>
-      <c r="N377" t="s">
-        <v>412</v>
-      </c>
+      <c r="N377"/>
       <c r="O377"/>
       <c r="P377"/>
       <c r="Q377"/>
       <c r="R377"/>
-      <c r="S377"/>
+      <c r="S377" t="s">
+        <v>412</v>
+      </c>
       <c r="T377"/>
       <c r="U377"/>
       <c r="V377"/>
@@ -18332,13 +18331,13 @@
         <v>413</v>
       </c>
       <c r="B378" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="C378" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="D378" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="E378" t="n">
         <v>5</v>
@@ -18349,16 +18348,16 @@
       <c r="I378"/>
       <c r="J378"/>
       <c r="K378"/>
-      <c r="L378"/>
+      <c r="L378" t="s">
+        <v>413</v>
+      </c>
       <c r="M378"/>
       <c r="N378"/>
       <c r="O378"/>
       <c r="P378"/>
       <c r="Q378"/>
       <c r="R378"/>
-      <c r="S378" t="s">
-        <v>413</v>
-      </c>
+      <c r="S378"/>
       <c r="T378"/>
       <c r="U378"/>
       <c r="V378"/>
@@ -18386,11 +18385,11 @@
       <c r="G379"/>
       <c r="H379"/>
       <c r="I379"/>
-      <c r="J379"/>
+      <c r="J379" t="s">
+        <v>414</v>
+      </c>
       <c r="K379"/>
-      <c r="L379" t="s">
-        <v>414</v>
-      </c>
+      <c r="L379"/>
       <c r="M379"/>
       <c r="N379"/>
       <c r="O379"/>
@@ -18410,13 +18409,13 @@
         <v>415</v>
       </c>
       <c r="B380" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C380" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D380" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E380" t="n">
         <v>5</v>
@@ -18425,16 +18424,16 @@
       <c r="G380"/>
       <c r="H380"/>
       <c r="I380"/>
-      <c r="J380" t="s">
-        <v>415</v>
-      </c>
+      <c r="J380"/>
       <c r="K380"/>
       <c r="L380"/>
       <c r="M380"/>
       <c r="N380"/>
       <c r="O380"/>
       <c r="P380"/>
-      <c r="Q380"/>
+      <c r="Q380" t="s">
+        <v>415</v>
+      </c>
       <c r="R380"/>
       <c r="S380"/>
       <c r="T380"/>
@@ -18468,12 +18467,12 @@
       <c r="K381"/>
       <c r="L381"/>
       <c r="M381"/>
-      <c r="N381"/>
+      <c r="N381" t="s">
+        <v>416</v>
+      </c>
       <c r="O381"/>
       <c r="P381"/>
-      <c r="Q381" t="s">
-        <v>416</v>
-      </c>
+      <c r="Q381"/>
       <c r="R381"/>
       <c r="S381"/>
       <c r="T381"/>
@@ -18488,13 +18487,13 @@
         <v>417</v>
       </c>
       <c r="B382" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C382" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D382" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E382" t="n">
         <v>5</v>
@@ -18505,11 +18504,11 @@
       <c r="I382"/>
       <c r="J382"/>
       <c r="K382"/>
-      <c r="L382"/>
+      <c r="L382" t="s">
+        <v>417</v>
+      </c>
       <c r="M382"/>
-      <c r="N382" t="s">
-        <v>417</v>
-      </c>
+      <c r="N382"/>
       <c r="O382"/>
       <c r="P382"/>
       <c r="Q382"/>
@@ -18566,13 +18565,13 @@
         <v>419</v>
       </c>
       <c r="B384" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="C384" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="D384" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="E384" t="n">
         <v>5</v>
@@ -18583,11 +18582,11 @@
       <c r="I384"/>
       <c r="J384"/>
       <c r="K384"/>
-      <c r="L384" t="s">
+      <c r="L384"/>
+      <c r="M384"/>
+      <c r="N384" t="s">
         <v>419</v>
       </c>
-      <c r="M384"/>
-      <c r="N384"/>
       <c r="O384"/>
       <c r="P384"/>
       <c r="Q384"/>
@@ -18644,13 +18643,13 @@
         <v>421</v>
       </c>
       <c r="B386" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="C386" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="D386" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="E386" t="n">
         <v>5</v>
@@ -18661,11 +18660,11 @@
       <c r="I386"/>
       <c r="J386"/>
       <c r="K386"/>
-      <c r="L386"/>
+      <c r="L386" t="s">
+        <v>421</v>
+      </c>
       <c r="M386"/>
-      <c r="N386" t="s">
-        <v>421</v>
-      </c>
+      <c r="N386"/>
       <c r="O386"/>
       <c r="P386"/>
       <c r="Q386"/>
@@ -18716,45 +18715,6 @@
       <c r="W387"/>
       <c r="X387"/>
       <c r="Y387"/>
-    </row>
-    <row r="388">
-      <c r="A388" t="s">
-        <v>423</v>
-      </c>
-      <c r="B388" t="s">
-        <v>26</v>
-      </c>
-      <c r="C388" t="s">
-        <v>26</v>
-      </c>
-      <c r="D388" t="s">
-        <v>26</v>
-      </c>
-      <c r="E388" t="n">
-        <v>5</v>
-      </c>
-      <c r="F388"/>
-      <c r="G388"/>
-      <c r="H388"/>
-      <c r="I388"/>
-      <c r="J388"/>
-      <c r="K388"/>
-      <c r="L388" t="s">
-        <v>423</v>
-      </c>
-      <c r="M388"/>
-      <c r="N388"/>
-      <c r="O388"/>
-      <c r="P388"/>
-      <c r="Q388"/>
-      <c r="R388"/>
-      <c r="S388"/>
-      <c r="T388"/>
-      <c r="U388"/>
-      <c r="V388"/>
-      <c r="W388"/>
-      <c r="X388"/>
-      <c r="Y388"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19438,7 +19398,9 @@
       <c r="G11" t="s">
         <v>26</v>
       </c>
-      <c r="H11"/>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
       <c r="I11" t="s">
         <v>26</v>
       </c>
@@ -27886,16 +27848,16 @@
       <c r="E259"/>
       <c r="F259"/>
       <c r="G259"/>
-      <c r="H259" t="s">
-        <v>26</v>
-      </c>
+      <c r="H259"/>
       <c r="I259"/>
       <c r="J259"/>
       <c r="K259"/>
       <c r="L259"/>
       <c r="M259"/>
       <c r="N259"/>
-      <c r="O259"/>
+      <c r="O259" t="s">
+        <v>26</v>
+      </c>
       <c r="P259"/>
       <c r="Q259"/>
       <c r="R259"/>
@@ -27920,14 +27882,14 @@
       <c r="L260"/>
       <c r="M260"/>
       <c r="N260"/>
-      <c r="O260" t="s">
-        <v>26</v>
-      </c>
+      <c r="O260"/>
       <c r="P260"/>
       <c r="Q260"/>
       <c r="R260"/>
       <c r="S260"/>
-      <c r="T260"/>
+      <c r="T260" t="s">
+        <v>29</v>
+      </c>
       <c r="U260"/>
     </row>
     <row r="261">
@@ -27936,7 +27898,9 @@
       </c>
       <c r="B261"/>
       <c r="C261"/>
-      <c r="D261"/>
+      <c r="D261" t="s">
+        <v>26</v>
+      </c>
       <c r="E261"/>
       <c r="F261"/>
       <c r="G261"/>
@@ -27952,9 +27916,7 @@
       <c r="Q261"/>
       <c r="R261"/>
       <c r="S261"/>
-      <c r="T261" t="s">
-        <v>29</v>
-      </c>
+      <c r="T261"/>
       <c r="U261"/>
     </row>
     <row r="262">
@@ -27964,7 +27926,7 @@
       <c r="B262"/>
       <c r="C262"/>
       <c r="D262" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="E262"/>
       <c r="F262"/>
@@ -27991,7 +27953,7 @@
       <c r="B263"/>
       <c r="C263"/>
       <c r="D263" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="E263"/>
       <c r="F263"/>
@@ -28017,9 +27979,7 @@
       </c>
       <c r="B264"/>
       <c r="C264"/>
-      <c r="D264" t="s">
-        <v>26</v>
-      </c>
+      <c r="D264"/>
       <c r="E264"/>
       <c r="F264"/>
       <c r="G264"/>
@@ -28028,7 +27988,9 @@
       <c r="J264"/>
       <c r="K264"/>
       <c r="L264"/>
-      <c r="M264"/>
+      <c r="M264" t="s">
+        <v>29</v>
+      </c>
       <c r="N264"/>
       <c r="O264"/>
       <c r="P264"/>
@@ -28049,13 +28011,13 @@
       <c r="F265"/>
       <c r="G265"/>
       <c r="H265"/>
-      <c r="I265"/>
+      <c r="I265" t="s">
+        <v>29</v>
+      </c>
       <c r="J265"/>
       <c r="K265"/>
       <c r="L265"/>
-      <c r="M265" t="s">
-        <v>29</v>
-      </c>
+      <c r="M265"/>
       <c r="N265"/>
       <c r="O265"/>
       <c r="P265"/>
@@ -28074,11 +28036,11 @@
       <c r="D266"/>
       <c r="E266"/>
       <c r="F266"/>
-      <c r="G266"/>
+      <c r="G266" t="s">
+        <v>29</v>
+      </c>
       <c r="H266"/>
-      <c r="I266" t="s">
-        <v>29</v>
-      </c>
+      <c r="I266"/>
       <c r="J266"/>
       <c r="K266"/>
       <c r="L266"/>
@@ -28101,16 +28063,16 @@
       <c r="D267"/>
       <c r="E267"/>
       <c r="F267"/>
-      <c r="G267" t="s">
-        <v>29</v>
-      </c>
+      <c r="G267"/>
       <c r="H267"/>
       <c r="I267"/>
       <c r="J267"/>
       <c r="K267"/>
       <c r="L267"/>
       <c r="M267"/>
-      <c r="N267"/>
+      <c r="N267" t="s">
+        <v>29</v>
+      </c>
       <c r="O267"/>
       <c r="P267"/>
       <c r="Q267"/>
@@ -28135,10 +28097,10 @@
       <c r="K268"/>
       <c r="L268"/>
       <c r="M268"/>
-      <c r="N268" t="s">
-        <v>29</v>
-      </c>
-      <c r="O268"/>
+      <c r="N268"/>
+      <c r="O268" t="s">
+        <v>29</v>
+      </c>
       <c r="P268"/>
       <c r="Q268"/>
       <c r="R268"/>
@@ -28158,14 +28120,14 @@
       <c r="G269"/>
       <c r="H269"/>
       <c r="I269"/>
-      <c r="J269"/>
+      <c r="J269" t="s">
+        <v>29</v>
+      </c>
       <c r="K269"/>
       <c r="L269"/>
       <c r="M269"/>
       <c r="N269"/>
-      <c r="O269" t="s">
-        <v>29</v>
-      </c>
+      <c r="O269"/>
       <c r="P269"/>
       <c r="Q269"/>
       <c r="R269"/>
@@ -28237,11 +28199,11 @@
       <c r="E272"/>
       <c r="F272"/>
       <c r="G272"/>
-      <c r="H272"/>
+      <c r="H272" t="s">
+        <v>29</v>
+      </c>
       <c r="I272"/>
-      <c r="J272" t="s">
-        <v>29</v>
-      </c>
+      <c r="J272"/>
       <c r="K272"/>
       <c r="L272"/>
       <c r="M272"/>
@@ -28264,11 +28226,11 @@
       <c r="E273"/>
       <c r="F273"/>
       <c r="G273"/>
-      <c r="H273" t="s">
-        <v>29</v>
-      </c>
+      <c r="H273"/>
       <c r="I273"/>
-      <c r="J273"/>
+      <c r="J273" t="s">
+        <v>29</v>
+      </c>
       <c r="K273"/>
       <c r="L273"/>
       <c r="M273"/>
@@ -28291,11 +28253,11 @@
       <c r="E274"/>
       <c r="F274"/>
       <c r="G274"/>
-      <c r="H274"/>
+      <c r="H274" t="s">
+        <v>29</v>
+      </c>
       <c r="I274"/>
-      <c r="J274" t="s">
-        <v>29</v>
-      </c>
+      <c r="J274"/>
       <c r="K274"/>
       <c r="L274"/>
       <c r="M274"/>
@@ -28318,16 +28280,16 @@
       <c r="E275"/>
       <c r="F275"/>
       <c r="G275"/>
-      <c r="H275" t="s">
-        <v>29</v>
-      </c>
+      <c r="H275"/>
       <c r="I275"/>
       <c r="J275"/>
       <c r="K275"/>
       <c r="L275"/>
       <c r="M275"/>
       <c r="N275"/>
-      <c r="O275"/>
+      <c r="O275" t="s">
+        <v>29</v>
+      </c>
       <c r="P275"/>
       <c r="Q275"/>
       <c r="R275"/>
@@ -28351,10 +28313,10 @@
       <c r="K276"/>
       <c r="L276"/>
       <c r="M276"/>
-      <c r="N276"/>
-      <c r="O276" t="s">
-        <v>29</v>
-      </c>
+      <c r="N276" t="s">
+        <v>29</v>
+      </c>
+      <c r="O276"/>
       <c r="P276"/>
       <c r="Q276"/>
       <c r="R276"/>
@@ -28368,7 +28330,9 @@
       </c>
       <c r="B277"/>
       <c r="C277"/>
-      <c r="D277"/>
+      <c r="D277" t="s">
+        <v>26</v>
+      </c>
       <c r="E277"/>
       <c r="F277"/>
       <c r="G277"/>
@@ -28378,9 +28342,7 @@
       <c r="K277"/>
       <c r="L277"/>
       <c r="M277"/>
-      <c r="N277" t="s">
-        <v>29</v>
-      </c>
+      <c r="N277"/>
       <c r="O277"/>
       <c r="P277"/>
       <c r="Q277"/>
@@ -28422,9 +28384,7 @@
       </c>
       <c r="B279"/>
       <c r="C279"/>
-      <c r="D279" t="s">
-        <v>26</v>
-      </c>
+      <c r="D279"/>
       <c r="E279"/>
       <c r="F279"/>
       <c r="G279"/>
@@ -28435,7 +28395,9 @@
       <c r="L279"/>
       <c r="M279"/>
       <c r="N279"/>
-      <c r="O279"/>
+      <c r="O279" t="s">
+        <v>26</v>
+      </c>
       <c r="P279"/>
       <c r="Q279"/>
       <c r="R279"/>
@@ -28459,10 +28421,10 @@
       <c r="K280"/>
       <c r="L280"/>
       <c r="M280"/>
-      <c r="N280"/>
-      <c r="O280" t="s">
-        <v>26</v>
-      </c>
+      <c r="N280" t="s">
+        <v>26</v>
+      </c>
+      <c r="O280"/>
       <c r="P280"/>
       <c r="Q280"/>
       <c r="R280"/>
@@ -28485,10 +28447,10 @@
       <c r="J281"/>
       <c r="K281"/>
       <c r="L281"/>
-      <c r="M281"/>
-      <c r="N281" t="s">
-        <v>26</v>
-      </c>
+      <c r="M281" t="s">
+        <v>26</v>
+      </c>
+      <c r="N281"/>
       <c r="O281"/>
       <c r="P281"/>
       <c r="Q281"/>
@@ -28534,14 +28496,14 @@
       <c r="E283"/>
       <c r="F283"/>
       <c r="G283"/>
-      <c r="H283"/>
+      <c r="H283" t="s">
+        <v>26</v>
+      </c>
       <c r="I283"/>
       <c r="J283"/>
       <c r="K283"/>
       <c r="L283"/>
-      <c r="M283" t="s">
-        <v>26</v>
-      </c>
+      <c r="M283"/>
       <c r="N283"/>
       <c r="O283"/>
       <c r="P283"/>
@@ -28561,16 +28523,16 @@
       <c r="E284"/>
       <c r="F284"/>
       <c r="G284"/>
-      <c r="H284" t="s">
-        <v>26</v>
-      </c>
+      <c r="H284"/>
       <c r="I284"/>
       <c r="J284"/>
       <c r="K284"/>
       <c r="L284"/>
       <c r="M284"/>
       <c r="N284"/>
-      <c r="O284"/>
+      <c r="O284" t="s">
+        <v>29</v>
+      </c>
       <c r="P284"/>
       <c r="Q284"/>
       <c r="R284"/>
@@ -28586,7 +28548,9 @@
       <c r="C285"/>
       <c r="D285"/>
       <c r="E285"/>
-      <c r="F285"/>
+      <c r="F285" t="s">
+        <v>26</v>
+      </c>
       <c r="G285"/>
       <c r="H285"/>
       <c r="I285"/>
@@ -28595,9 +28559,7 @@
       <c r="L285"/>
       <c r="M285"/>
       <c r="N285"/>
-      <c r="O285" t="s">
-        <v>29</v>
-      </c>
+      <c r="O285"/>
       <c r="P285"/>
       <c r="Q285"/>
       <c r="R285"/>
@@ -28613,11 +28575,11 @@
       <c r="C286"/>
       <c r="D286"/>
       <c r="E286"/>
-      <c r="F286" t="s">
-        <v>26</v>
-      </c>
+      <c r="F286"/>
       <c r="G286"/>
-      <c r="H286"/>
+      <c r="H286" t="s">
+        <v>26</v>
+      </c>
       <c r="I286"/>
       <c r="J286"/>
       <c r="K286"/>
@@ -28666,12 +28628,12 @@
       <c r="B288"/>
       <c r="C288"/>
       <c r="D288"/>
-      <c r="E288"/>
+      <c r="E288" t="s">
+        <v>26</v>
+      </c>
       <c r="F288"/>
       <c r="G288"/>
-      <c r="H288" t="s">
-        <v>26</v>
-      </c>
+      <c r="H288"/>
       <c r="I288"/>
       <c r="J288"/>
       <c r="K288"/>
@@ -28693,14 +28655,14 @@
       <c r="B289"/>
       <c r="C289"/>
       <c r="D289"/>
-      <c r="E289" t="s">
-        <v>26</v>
-      </c>
+      <c r="E289"/>
       <c r="F289"/>
       <c r="G289"/>
       <c r="H289"/>
       <c r="I289"/>
-      <c r="J289"/>
+      <c r="J289" t="s">
+        <v>29</v>
+      </c>
       <c r="K289"/>
       <c r="L289"/>
       <c r="M289"/>
@@ -28751,10 +28713,10 @@
       <c r="F291"/>
       <c r="G291"/>
       <c r="H291"/>
-      <c r="I291"/>
-      <c r="J291" t="s">
-        <v>29</v>
-      </c>
+      <c r="I291" t="s">
+        <v>56</v>
+      </c>
+      <c r="J291"/>
       <c r="K291"/>
       <c r="L291"/>
       <c r="M291"/>
@@ -28777,10 +28739,10 @@
       <c r="E292"/>
       <c r="F292"/>
       <c r="G292"/>
-      <c r="H292"/>
-      <c r="I292" t="s">
+      <c r="H292" t="s">
         <v>56</v>
       </c>
+      <c r="I292"/>
       <c r="J292"/>
       <c r="K292"/>
       <c r="L292"/>
@@ -28804,16 +28766,16 @@
       <c r="E293"/>
       <c r="F293"/>
       <c r="G293"/>
-      <c r="H293" t="s">
-        <v>56</v>
-      </c>
+      <c r="H293"/>
       <c r="I293"/>
       <c r="J293"/>
       <c r="K293"/>
       <c r="L293"/>
       <c r="M293"/>
       <c r="N293"/>
-      <c r="O293"/>
+      <c r="O293" t="s">
+        <v>88</v>
+      </c>
       <c r="P293"/>
       <c r="Q293"/>
       <c r="R293"/>
@@ -28833,14 +28795,14 @@
       <c r="G294"/>
       <c r="H294"/>
       <c r="I294"/>
-      <c r="J294"/>
+      <c r="J294" t="s">
+        <v>29</v>
+      </c>
       <c r="K294"/>
       <c r="L294"/>
       <c r="M294"/>
       <c r="N294"/>
-      <c r="O294" t="s">
-        <v>88</v>
-      </c>
+      <c r="O294"/>
       <c r="P294"/>
       <c r="Q294"/>
       <c r="R294"/>
@@ -28914,14 +28876,14 @@
       <c r="G297"/>
       <c r="H297"/>
       <c r="I297"/>
-      <c r="J297" t="s">
-        <v>29</v>
-      </c>
+      <c r="J297"/>
       <c r="K297"/>
       <c r="L297"/>
       <c r="M297"/>
       <c r="N297"/>
-      <c r="O297"/>
+      <c r="O297" t="s">
+        <v>56</v>
+      </c>
       <c r="P297"/>
       <c r="Q297"/>
       <c r="R297"/>
@@ -28935,7 +28897,9 @@
       </c>
       <c r="B298"/>
       <c r="C298"/>
-      <c r="D298"/>
+      <c r="D298" t="s">
+        <v>26</v>
+      </c>
       <c r="E298"/>
       <c r="F298"/>
       <c r="G298"/>
@@ -28946,9 +28910,7 @@
       <c r="L298"/>
       <c r="M298"/>
       <c r="N298"/>
-      <c r="O298" t="s">
-        <v>56</v>
-      </c>
+      <c r="O298"/>
       <c r="P298"/>
       <c r="Q298"/>
       <c r="R298"/>
@@ -28962,13 +28924,13 @@
       </c>
       <c r="B299"/>
       <c r="C299"/>
-      <c r="D299" t="s">
-        <v>26</v>
-      </c>
+      <c r="D299"/>
       <c r="E299"/>
       <c r="F299"/>
       <c r="G299"/>
-      <c r="H299"/>
+      <c r="H299" t="s">
+        <v>26</v>
+      </c>
       <c r="I299"/>
       <c r="J299"/>
       <c r="K299"/>
@@ -28993,14 +28955,14 @@
       <c r="E300"/>
       <c r="F300"/>
       <c r="G300"/>
-      <c r="H300" t="s">
-        <v>26</v>
-      </c>
+      <c r="H300"/>
       <c r="I300"/>
       <c r="J300"/>
       <c r="K300"/>
       <c r="L300"/>
-      <c r="M300"/>
+      <c r="M300" t="s">
+        <v>29</v>
+      </c>
       <c r="N300"/>
       <c r="O300"/>
       <c r="P300"/>
@@ -29026,7 +28988,7 @@
       <c r="K301"/>
       <c r="L301"/>
       <c r="M301" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N301"/>
       <c r="O301"/>
@@ -29045,16 +29007,16 @@
       <c r="C302"/>
       <c r="D302"/>
       <c r="E302"/>
-      <c r="F302"/>
+      <c r="F302" t="s">
+        <v>26</v>
+      </c>
       <c r="G302"/>
       <c r="H302"/>
       <c r="I302"/>
       <c r="J302"/>
       <c r="K302"/>
       <c r="L302"/>
-      <c r="M302" t="s">
-        <v>26</v>
-      </c>
+      <c r="M302"/>
       <c r="N302"/>
       <c r="O302"/>
       <c r="P302"/>
@@ -29072,11 +29034,11 @@
       <c r="C303"/>
       <c r="D303"/>
       <c r="E303"/>
-      <c r="F303" t="s">
-        <v>26</v>
-      </c>
+      <c r="F303"/>
       <c r="G303"/>
-      <c r="H303"/>
+      <c r="H303" t="s">
+        <v>26</v>
+      </c>
       <c r="I303"/>
       <c r="J303"/>
       <c r="K303"/>
@@ -29128,9 +29090,7 @@
       <c r="E305"/>
       <c r="F305"/>
       <c r="G305"/>
-      <c r="H305" t="s">
-        <v>26</v>
-      </c>
+      <c r="H305"/>
       <c r="I305"/>
       <c r="J305"/>
       <c r="K305"/>
@@ -29141,7 +29101,9 @@
       <c r="P305"/>
       <c r="Q305"/>
       <c r="R305"/>
-      <c r="S305"/>
+      <c r="S305" t="s">
+        <v>26</v>
+      </c>
       <c r="T305"/>
       <c r="U305"/>
     </row>
@@ -29151,7 +29113,9 @@
       </c>
       <c r="B306"/>
       <c r="C306"/>
-      <c r="D306"/>
+      <c r="D306" t="s">
+        <v>29</v>
+      </c>
       <c r="E306"/>
       <c r="F306"/>
       <c r="G306"/>
@@ -29166,9 +29130,7 @@
       <c r="P306"/>
       <c r="Q306"/>
       <c r="R306"/>
-      <c r="S306" t="s">
-        <v>26</v>
-      </c>
+      <c r="S306"/>
       <c r="T306"/>
       <c r="U306"/>
     </row>
@@ -29178,9 +29140,7 @@
       </c>
       <c r="B307"/>
       <c r="C307"/>
-      <c r="D307" t="s">
-        <v>29</v>
-      </c>
+      <c r="D307"/>
       <c r="E307"/>
       <c r="F307"/>
       <c r="G307"/>
@@ -29190,7 +29150,9 @@
       <c r="K307"/>
       <c r="L307"/>
       <c r="M307"/>
-      <c r="N307"/>
+      <c r="N307" t="s">
+        <v>29</v>
+      </c>
       <c r="O307"/>
       <c r="P307"/>
       <c r="Q307"/>
@@ -29209,15 +29171,15 @@
       <c r="E308"/>
       <c r="F308"/>
       <c r="G308"/>
-      <c r="H308"/>
+      <c r="H308" t="s">
+        <v>88</v>
+      </c>
       <c r="I308"/>
       <c r="J308"/>
       <c r="K308"/>
       <c r="L308"/>
       <c r="M308"/>
-      <c r="N308" t="s">
-        <v>29</v>
-      </c>
+      <c r="N308"/>
       <c r="O308"/>
       <c r="P308"/>
       <c r="Q308"/>
@@ -29236,11 +29198,11 @@
       <c r="E309"/>
       <c r="F309"/>
       <c r="G309"/>
-      <c r="H309" t="s">
-        <v>88</v>
-      </c>
+      <c r="H309"/>
       <c r="I309"/>
-      <c r="J309"/>
+      <c r="J309" t="s">
+        <v>26</v>
+      </c>
       <c r="K309"/>
       <c r="L309"/>
       <c r="M309"/>
@@ -29265,10 +29227,10 @@
       <c r="G310"/>
       <c r="H310"/>
       <c r="I310"/>
-      <c r="J310" t="s">
-        <v>26</v>
-      </c>
-      <c r="K310"/>
+      <c r="J310"/>
+      <c r="K310" t="s">
+        <v>26</v>
+      </c>
       <c r="L310"/>
       <c r="M310"/>
       <c r="N310"/>
@@ -29290,12 +29252,12 @@
       <c r="E311"/>
       <c r="F311"/>
       <c r="G311"/>
-      <c r="H311"/>
+      <c r="H311" t="s">
+        <v>56</v>
+      </c>
       <c r="I311"/>
       <c r="J311"/>
-      <c r="K311" t="s">
-        <v>26</v>
-      </c>
+      <c r="K311"/>
       <c r="L311"/>
       <c r="M311"/>
       <c r="N311"/>
@@ -29314,12 +29276,12 @@
       <c r="B312"/>
       <c r="C312"/>
       <c r="D312"/>
-      <c r="E312"/>
+      <c r="E312" t="s">
+        <v>29</v>
+      </c>
       <c r="F312"/>
       <c r="G312"/>
-      <c r="H312" t="s">
-        <v>56</v>
-      </c>
+      <c r="H312"/>
       <c r="I312"/>
       <c r="J312"/>
       <c r="K312"/>
@@ -29341,10 +29303,10 @@
       <c r="B313"/>
       <c r="C313"/>
       <c r="D313"/>
-      <c r="E313" t="s">
-        <v>29</v>
-      </c>
-      <c r="F313"/>
+      <c r="E313"/>
+      <c r="F313" t="s">
+        <v>29</v>
+      </c>
       <c r="G313"/>
       <c r="H313"/>
       <c r="I313"/>
@@ -29367,11 +29329,11 @@
       </c>
       <c r="B314"/>
       <c r="C314"/>
-      <c r="D314"/>
+      <c r="D314" t="s">
+        <v>29</v>
+      </c>
       <c r="E314"/>
-      <c r="F314" t="s">
-        <v>29</v>
-      </c>
+      <c r="F314"/>
       <c r="G314"/>
       <c r="H314"/>
       <c r="I314"/>
@@ -29395,7 +29357,7 @@
       <c r="B315"/>
       <c r="C315"/>
       <c r="D315" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E315"/>
       <c r="F315"/>
@@ -29421,13 +29383,13 @@
       </c>
       <c r="B316"/>
       <c r="C316"/>
-      <c r="D316" t="s">
-        <v>26</v>
-      </c>
+      <c r="D316"/>
       <c r="E316"/>
       <c r="F316"/>
       <c r="G316"/>
-      <c r="H316"/>
+      <c r="H316" t="s">
+        <v>26</v>
+      </c>
       <c r="I316"/>
       <c r="J316"/>
       <c r="K316"/>
@@ -29476,12 +29438,12 @@
       <c r="B318"/>
       <c r="C318"/>
       <c r="D318"/>
-      <c r="E318"/>
+      <c r="E318" t="s">
+        <v>29</v>
+      </c>
       <c r="F318"/>
       <c r="G318"/>
-      <c r="H318" t="s">
-        <v>26</v>
-      </c>
+      <c r="H318"/>
       <c r="I318"/>
       <c r="J318"/>
       <c r="K318"/>
@@ -29503,10 +29465,10 @@
       <c r="B319"/>
       <c r="C319"/>
       <c r="D319"/>
-      <c r="E319" t="s">
-        <v>29</v>
-      </c>
-      <c r="F319"/>
+      <c r="E319"/>
+      <c r="F319" t="s">
+        <v>29</v>
+      </c>
       <c r="G319"/>
       <c r="H319"/>
       <c r="I319"/>
@@ -29529,11 +29491,11 @@
       </c>
       <c r="B320"/>
       <c r="C320"/>
-      <c r="D320"/>
+      <c r="D320" t="s">
+        <v>29</v>
+      </c>
       <c r="E320"/>
-      <c r="F320" t="s">
-        <v>29</v>
-      </c>
+      <c r="F320"/>
       <c r="G320"/>
       <c r="H320"/>
       <c r="I320"/>
@@ -29556,9 +29518,7 @@
       </c>
       <c r="B321"/>
       <c r="C321"/>
-      <c r="D321" t="s">
-        <v>29</v>
-      </c>
+      <c r="D321"/>
       <c r="E321"/>
       <c r="F321"/>
       <c r="G321"/>
@@ -29567,7 +29527,9 @@
       <c r="J321"/>
       <c r="K321"/>
       <c r="L321"/>
-      <c r="M321"/>
+      <c r="M321" t="s">
+        <v>26</v>
+      </c>
       <c r="N321"/>
       <c r="O321"/>
       <c r="P321"/>
@@ -29592,11 +29554,11 @@
       <c r="J322"/>
       <c r="K322"/>
       <c r="L322"/>
-      <c r="M322" t="s">
-        <v>26</v>
-      </c>
+      <c r="M322"/>
       <c r="N322"/>
-      <c r="O322"/>
+      <c r="O322" t="s">
+        <v>29</v>
+      </c>
       <c r="P322"/>
       <c r="Q322"/>
       <c r="R322"/>
@@ -29619,11 +29581,11 @@
       <c r="J323"/>
       <c r="K323"/>
       <c r="L323"/>
-      <c r="M323"/>
+      <c r="M323" t="s">
+        <v>29</v>
+      </c>
       <c r="N323"/>
-      <c r="O323" t="s">
-        <v>29</v>
-      </c>
+      <c r="O323"/>
       <c r="P323"/>
       <c r="Q323"/>
       <c r="R323"/>
@@ -29673,11 +29635,11 @@
       <c r="J325"/>
       <c r="K325"/>
       <c r="L325"/>
-      <c r="M325" t="s">
-        <v>29</v>
-      </c>
+      <c r="M325"/>
       <c r="N325"/>
-      <c r="O325"/>
+      <c r="O325" t="s">
+        <v>26</v>
+      </c>
       <c r="P325"/>
       <c r="Q325"/>
       <c r="R325"/>
@@ -29693,7 +29655,9 @@
       <c r="C326"/>
       <c r="D326"/>
       <c r="E326"/>
-      <c r="F326"/>
+      <c r="F326" t="s">
+        <v>26</v>
+      </c>
       <c r="G326"/>
       <c r="H326"/>
       <c r="I326"/>
@@ -29702,9 +29666,7 @@
       <c r="L326"/>
       <c r="M326"/>
       <c r="N326"/>
-      <c r="O326" t="s">
-        <v>26</v>
-      </c>
+      <c r="O326"/>
       <c r="P326"/>
       <c r="Q326"/>
       <c r="R326"/>
@@ -29720,14 +29682,14 @@
       <c r="C327"/>
       <c r="D327"/>
       <c r="E327"/>
-      <c r="F327" t="s">
-        <v>26</v>
-      </c>
+      <c r="F327"/>
       <c r="G327"/>
       <c r="H327"/>
       <c r="I327"/>
       <c r="J327"/>
-      <c r="K327"/>
+      <c r="K327" t="s">
+        <v>29</v>
+      </c>
       <c r="L327"/>
       <c r="M327"/>
       <c r="N327"/>
@@ -29747,14 +29709,14 @@
       <c r="C328"/>
       <c r="D328"/>
       <c r="E328"/>
-      <c r="F328"/>
+      <c r="F328" t="s">
+        <v>26</v>
+      </c>
       <c r="G328"/>
       <c r="H328"/>
       <c r="I328"/>
       <c r="J328"/>
-      <c r="K328" t="s">
-        <v>29</v>
-      </c>
+      <c r="K328"/>
       <c r="L328"/>
       <c r="M328"/>
       <c r="N328"/>
@@ -29774,9 +29736,7 @@
       <c r="C329"/>
       <c r="D329"/>
       <c r="E329"/>
-      <c r="F329" t="s">
-        <v>26</v>
-      </c>
+      <c r="F329"/>
       <c r="G329"/>
       <c r="H329"/>
       <c r="I329"/>
@@ -29784,7 +29744,9 @@
       <c r="K329"/>
       <c r="L329"/>
       <c r="M329"/>
-      <c r="N329"/>
+      <c r="N329" t="s">
+        <v>26</v>
+      </c>
       <c r="O329"/>
       <c r="P329"/>
       <c r="Q329"/>
@@ -29800,7 +29762,9 @@
       <c r="B330"/>
       <c r="C330"/>
       <c r="D330"/>
-      <c r="E330"/>
+      <c r="E330" t="s">
+        <v>26</v>
+      </c>
       <c r="F330"/>
       <c r="G330"/>
       <c r="H330"/>
@@ -29809,9 +29773,7 @@
       <c r="K330"/>
       <c r="L330"/>
       <c r="M330"/>
-      <c r="N330" t="s">
-        <v>26</v>
-      </c>
+      <c r="N330"/>
       <c r="O330"/>
       <c r="P330"/>
       <c r="Q330"/>
@@ -29826,10 +29788,10 @@
       </c>
       <c r="B331"/>
       <c r="C331"/>
-      <c r="D331"/>
-      <c r="E331" t="s">
-        <v>26</v>
-      </c>
+      <c r="D331" t="s">
+        <v>26</v>
+      </c>
+      <c r="E331"/>
       <c r="F331"/>
       <c r="G331"/>
       <c r="H331"/>
@@ -29961,13 +29923,13 @@
       </c>
       <c r="B336"/>
       <c r="C336"/>
-      <c r="D336" t="s">
-        <v>26</v>
-      </c>
+      <c r="D336"/>
       <c r="E336"/>
       <c r="F336"/>
       <c r="G336"/>
-      <c r="H336"/>
+      <c r="H336" t="s">
+        <v>26</v>
+      </c>
       <c r="I336"/>
       <c r="J336"/>
       <c r="K336"/>
@@ -29992,11 +29954,11 @@
       <c r="E337"/>
       <c r="F337"/>
       <c r="G337"/>
-      <c r="H337" t="s">
-        <v>26</v>
-      </c>
+      <c r="H337"/>
       <c r="I337"/>
-      <c r="J337"/>
+      <c r="J337" t="s">
+        <v>29</v>
+      </c>
       <c r="K337"/>
       <c r="L337"/>
       <c r="M337"/>
@@ -30021,13 +29983,13 @@
       <c r="G338"/>
       <c r="H338"/>
       <c r="I338"/>
-      <c r="J338" t="s">
-        <v>29</v>
-      </c>
+      <c r="J338"/>
       <c r="K338"/>
       <c r="L338"/>
       <c r="M338"/>
-      <c r="N338"/>
+      <c r="N338" t="s">
+        <v>26</v>
+      </c>
       <c r="O338"/>
       <c r="P338"/>
       <c r="Q338"/>
@@ -30042,7 +30004,9 @@
       </c>
       <c r="B339"/>
       <c r="C339"/>
-      <c r="D339"/>
+      <c r="D339" t="s">
+        <v>26</v>
+      </c>
       <c r="E339"/>
       <c r="F339"/>
       <c r="G339"/>
@@ -30052,9 +30016,7 @@
       <c r="K339"/>
       <c r="L339"/>
       <c r="M339"/>
-      <c r="N339" t="s">
-        <v>26</v>
-      </c>
+      <c r="N339"/>
       <c r="O339"/>
       <c r="P339"/>
       <c r="Q339"/>
@@ -30096,10 +30058,10 @@
       </c>
       <c r="B341"/>
       <c r="C341"/>
-      <c r="D341" t="s">
-        <v>26</v>
-      </c>
-      <c r="E341"/>
+      <c r="D341"/>
+      <c r="E341" t="s">
+        <v>26</v>
+      </c>
       <c r="F341"/>
       <c r="G341"/>
       <c r="H341"/>
@@ -30124,12 +30086,12 @@
       <c r="B342"/>
       <c r="C342"/>
       <c r="D342"/>
-      <c r="E342" t="s">
-        <v>26</v>
-      </c>
+      <c r="E342"/>
       <c r="F342"/>
       <c r="G342"/>
-      <c r="H342"/>
+      <c r="H342" t="s">
+        <v>26</v>
+      </c>
       <c r="I342"/>
       <c r="J342"/>
       <c r="K342"/>
@@ -30154,15 +30116,15 @@
       <c r="E343"/>
       <c r="F343"/>
       <c r="G343"/>
-      <c r="H343" t="s">
-        <v>26</v>
-      </c>
+      <c r="H343"/>
       <c r="I343"/>
       <c r="J343"/>
       <c r="K343"/>
       <c r="L343"/>
       <c r="M343"/>
-      <c r="N343"/>
+      <c r="N343" t="s">
+        <v>26</v>
+      </c>
       <c r="O343"/>
       <c r="P343"/>
       <c r="Q343"/>
@@ -30183,13 +30145,13 @@
       <c r="G344"/>
       <c r="H344"/>
       <c r="I344"/>
-      <c r="J344"/>
+      <c r="J344" t="s">
+        <v>26</v>
+      </c>
       <c r="K344"/>
       <c r="L344"/>
       <c r="M344"/>
-      <c r="N344" t="s">
-        <v>26</v>
-      </c>
+      <c r="N344"/>
       <c r="O344"/>
       <c r="P344"/>
       <c r="Q344"/>
@@ -30237,14 +30199,14 @@
       <c r="G346"/>
       <c r="H346"/>
       <c r="I346"/>
-      <c r="J346" t="s">
-        <v>26</v>
-      </c>
+      <c r="J346"/>
       <c r="K346"/>
       <c r="L346"/>
       <c r="M346"/>
       <c r="N346"/>
-      <c r="O346"/>
+      <c r="O346" t="s">
+        <v>26</v>
+      </c>
       <c r="P346"/>
       <c r="Q346"/>
       <c r="R346"/>
@@ -30289,16 +30251,16 @@
       <c r="E348"/>
       <c r="F348"/>
       <c r="G348"/>
-      <c r="H348"/>
+      <c r="H348" t="s">
+        <v>26</v>
+      </c>
       <c r="I348"/>
       <c r="J348"/>
       <c r="K348"/>
       <c r="L348"/>
       <c r="M348"/>
       <c r="N348"/>
-      <c r="O348" t="s">
-        <v>26</v>
-      </c>
+      <c r="O348"/>
       <c r="P348"/>
       <c r="Q348"/>
       <c r="R348"/>
@@ -30314,11 +30276,11 @@
       <c r="C349"/>
       <c r="D349"/>
       <c r="E349"/>
-      <c r="F349"/>
+      <c r="F349" t="s">
+        <v>26</v>
+      </c>
       <c r="G349"/>
-      <c r="H349" t="s">
-        <v>26</v>
-      </c>
+      <c r="H349"/>
       <c r="I349"/>
       <c r="J349"/>
       <c r="K349"/>
@@ -30341,11 +30303,11 @@
       <c r="C350"/>
       <c r="D350"/>
       <c r="E350"/>
-      <c r="F350" t="s">
-        <v>26</v>
-      </c>
+      <c r="F350"/>
       <c r="G350"/>
-      <c r="H350"/>
+      <c r="H350" t="s">
+        <v>26</v>
+      </c>
       <c r="I350"/>
       <c r="J350"/>
       <c r="K350"/>
@@ -30368,11 +30330,11 @@
       <c r="C351"/>
       <c r="D351"/>
       <c r="E351"/>
-      <c r="F351"/>
+      <c r="F351" t="s">
+        <v>26</v>
+      </c>
       <c r="G351"/>
-      <c r="H351" t="s">
-        <v>26</v>
-      </c>
+      <c r="H351"/>
       <c r="I351"/>
       <c r="J351"/>
       <c r="K351"/>
@@ -30395,13 +30357,13 @@
       <c r="C352"/>
       <c r="D352"/>
       <c r="E352"/>
-      <c r="F352" t="s">
-        <v>26</v>
-      </c>
+      <c r="F352"/>
       <c r="G352"/>
       <c r="H352"/>
       <c r="I352"/>
-      <c r="J352"/>
+      <c r="J352" t="s">
+        <v>29</v>
+      </c>
       <c r="K352"/>
       <c r="L352"/>
       <c r="M352"/>
@@ -30426,12 +30388,12 @@
       <c r="G353"/>
       <c r="H353"/>
       <c r="I353"/>
-      <c r="J353" t="s">
-        <v>29</v>
-      </c>
+      <c r="J353"/>
       <c r="K353"/>
       <c r="L353"/>
-      <c r="M353"/>
+      <c r="M353" t="s">
+        <v>29</v>
+      </c>
       <c r="N353"/>
       <c r="O353"/>
       <c r="P353"/>
@@ -30453,12 +30415,12 @@
       <c r="G354"/>
       <c r="H354"/>
       <c r="I354"/>
-      <c r="J354"/>
+      <c r="J354" t="s">
+        <v>26</v>
+      </c>
       <c r="K354"/>
       <c r="L354"/>
-      <c r="M354" t="s">
-        <v>29</v>
-      </c>
+      <c r="M354"/>
       <c r="N354"/>
       <c r="O354"/>
       <c r="P354"/>
@@ -30476,13 +30438,13 @@
       <c r="C355"/>
       <c r="D355"/>
       <c r="E355"/>
-      <c r="F355"/>
+      <c r="F355" t="s">
+        <v>26</v>
+      </c>
       <c r="G355"/>
       <c r="H355"/>
       <c r="I355"/>
-      <c r="J355" t="s">
-        <v>26</v>
-      </c>
+      <c r="J355"/>
       <c r="K355"/>
       <c r="L355"/>
       <c r="M355"/>
@@ -30503,9 +30465,7 @@
       <c r="C356"/>
       <c r="D356"/>
       <c r="E356"/>
-      <c r="F356" t="s">
-        <v>26</v>
-      </c>
+      <c r="F356"/>
       <c r="G356"/>
       <c r="H356"/>
       <c r="I356"/>
@@ -30514,7 +30474,9 @@
       <c r="L356"/>
       <c r="M356"/>
       <c r="N356"/>
-      <c r="O356"/>
+      <c r="O356" t="s">
+        <v>88</v>
+      </c>
       <c r="P356"/>
       <c r="Q356"/>
       <c r="R356"/>
@@ -30540,7 +30502,7 @@
       <c r="M357"/>
       <c r="N357"/>
       <c r="O357" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="P357"/>
       <c r="Q357"/>
@@ -30559,16 +30521,16 @@
       <c r="E358"/>
       <c r="F358"/>
       <c r="G358"/>
-      <c r="H358"/>
+      <c r="H358" t="s">
+        <v>26</v>
+      </c>
       <c r="I358"/>
       <c r="J358"/>
       <c r="K358"/>
       <c r="L358"/>
       <c r="M358"/>
       <c r="N358"/>
-      <c r="O358" t="s">
-        <v>29</v>
-      </c>
+      <c r="O358"/>
       <c r="P358"/>
       <c r="Q358"/>
       <c r="R358"/>
@@ -30640,9 +30602,7 @@
       <c r="E361"/>
       <c r="F361"/>
       <c r="G361"/>
-      <c r="H361" t="s">
-        <v>26</v>
-      </c>
+      <c r="H361"/>
       <c r="I361"/>
       <c r="J361"/>
       <c r="K361"/>
@@ -30650,7 +30610,9 @@
       <c r="M361"/>
       <c r="N361"/>
       <c r="O361"/>
-      <c r="P361"/>
+      <c r="P361" t="s">
+        <v>29</v>
+      </c>
       <c r="Q361"/>
       <c r="R361"/>
       <c r="S361"/>
@@ -30671,13 +30633,13 @@
       <c r="I362"/>
       <c r="J362"/>
       <c r="K362"/>
-      <c r="L362"/>
+      <c r="L362" t="s">
+        <v>29</v>
+      </c>
       <c r="M362"/>
       <c r="N362"/>
       <c r="O362"/>
-      <c r="P362" t="s">
-        <v>29</v>
-      </c>
+      <c r="P362"/>
       <c r="Q362"/>
       <c r="R362"/>
       <c r="S362"/>
@@ -30698,11 +30660,11 @@
       <c r="I363"/>
       <c r="J363"/>
       <c r="K363"/>
-      <c r="L363" t="s">
-        <v>29</v>
-      </c>
+      <c r="L363"/>
       <c r="M363"/>
-      <c r="N363"/>
+      <c r="N363" t="s">
+        <v>88</v>
+      </c>
       <c r="O363"/>
       <c r="P363"/>
       <c r="Q363"/>
@@ -30727,12 +30689,12 @@
       <c r="K364"/>
       <c r="L364"/>
       <c r="M364"/>
-      <c r="N364" t="s">
-        <v>88</v>
-      </c>
+      <c r="N364"/>
       <c r="O364"/>
       <c r="P364"/>
-      <c r="Q364"/>
+      <c r="Q364" t="s">
+        <v>26</v>
+      </c>
       <c r="R364"/>
       <c r="S364"/>
       <c r="T364"/>
@@ -30752,14 +30714,14 @@
       <c r="I365"/>
       <c r="J365"/>
       <c r="K365"/>
-      <c r="L365"/>
+      <c r="L365" t="s">
+        <v>26</v>
+      </c>
       <c r="M365"/>
       <c r="N365"/>
       <c r="O365"/>
       <c r="P365"/>
-      <c r="Q365" t="s">
-        <v>26</v>
-      </c>
+      <c r="Q365"/>
       <c r="R365"/>
       <c r="S365"/>
       <c r="T365"/>
@@ -30777,11 +30739,11 @@
       <c r="G366"/>
       <c r="H366"/>
       <c r="I366"/>
-      <c r="J366"/>
+      <c r="J366" t="s">
+        <v>26</v>
+      </c>
       <c r="K366"/>
-      <c r="L366" t="s">
-        <v>26</v>
-      </c>
+      <c r="L366"/>
       <c r="M366"/>
       <c r="N366"/>
       <c r="O366"/>
@@ -30804,14 +30766,14 @@
       <c r="G367"/>
       <c r="H367"/>
       <c r="I367"/>
-      <c r="J367" t="s">
-        <v>26</v>
-      </c>
+      <c r="J367"/>
       <c r="K367"/>
       <c r="L367"/>
       <c r="M367"/>
       <c r="N367"/>
-      <c r="O367"/>
+      <c r="O367" t="s">
+        <v>26</v>
+      </c>
       <c r="P367"/>
       <c r="Q367"/>
       <c r="R367"/>
@@ -30835,10 +30797,10 @@
       <c r="K368"/>
       <c r="L368"/>
       <c r="M368"/>
-      <c r="N368"/>
-      <c r="O368" t="s">
-        <v>26</v>
-      </c>
+      <c r="N368" t="s">
+        <v>26</v>
+      </c>
+      <c r="O368"/>
       <c r="P368"/>
       <c r="Q368"/>
       <c r="R368"/>
@@ -30859,12 +30821,12 @@
       <c r="H369"/>
       <c r="I369"/>
       <c r="J369"/>
-      <c r="K369"/>
+      <c r="K369" t="s">
+        <v>26</v>
+      </c>
       <c r="L369"/>
       <c r="M369"/>
-      <c r="N369" t="s">
-        <v>26</v>
-      </c>
+      <c r="N369"/>
       <c r="O369"/>
       <c r="P369"/>
       <c r="Q369"/>
@@ -30881,14 +30843,14 @@
       <c r="C370"/>
       <c r="D370"/>
       <c r="E370"/>
-      <c r="F370"/>
+      <c r="F370" t="s">
+        <v>26</v>
+      </c>
       <c r="G370"/>
       <c r="H370"/>
       <c r="I370"/>
       <c r="J370"/>
-      <c r="K370" t="s">
-        <v>26</v>
-      </c>
+      <c r="K370"/>
       <c r="L370"/>
       <c r="M370"/>
       <c r="N370"/>
@@ -30908,11 +30870,11 @@
       <c r="C371"/>
       <c r="D371"/>
       <c r="E371"/>
-      <c r="F371" t="s">
-        <v>26</v>
-      </c>
+      <c r="F371"/>
       <c r="G371"/>
-      <c r="H371"/>
+      <c r="H371" t="s">
+        <v>26</v>
+      </c>
       <c r="I371"/>
       <c r="J371"/>
       <c r="K371"/>
@@ -30937,11 +30899,11 @@
       <c r="E372"/>
       <c r="F372"/>
       <c r="G372"/>
-      <c r="H372" t="s">
-        <v>26</v>
-      </c>
+      <c r="H372"/>
       <c r="I372"/>
-      <c r="J372"/>
+      <c r="J372" t="s">
+        <v>26</v>
+      </c>
       <c r="K372"/>
       <c r="L372"/>
       <c r="M372"/>
@@ -30960,15 +30922,15 @@
       </c>
       <c r="B373"/>
       <c r="C373"/>
-      <c r="D373"/>
+      <c r="D373" t="s">
+        <v>26</v>
+      </c>
       <c r="E373"/>
       <c r="F373"/>
       <c r="G373"/>
       <c r="H373"/>
       <c r="I373"/>
-      <c r="J373" t="s">
-        <v>26</v>
-      </c>
+      <c r="J373"/>
       <c r="K373"/>
       <c r="L373"/>
       <c r="M373"/>
@@ -31014,9 +30976,7 @@
       </c>
       <c r="B375"/>
       <c r="C375"/>
-      <c r="D375" t="s">
-        <v>26</v>
-      </c>
+      <c r="D375"/>
       <c r="E375"/>
       <c r="F375"/>
       <c r="G375"/>
@@ -31026,7 +30986,9 @@
       <c r="K375"/>
       <c r="L375"/>
       <c r="M375"/>
-      <c r="N375"/>
+      <c r="N375" t="s">
+        <v>26</v>
+      </c>
       <c r="O375"/>
       <c r="P375"/>
       <c r="Q375"/>
@@ -31047,13 +31009,13 @@
       <c r="G376"/>
       <c r="H376"/>
       <c r="I376"/>
-      <c r="J376"/>
+      <c r="J376" t="s">
+        <v>26</v>
+      </c>
       <c r="K376"/>
       <c r="L376"/>
       <c r="M376"/>
-      <c r="N376" t="s">
-        <v>26</v>
-      </c>
+      <c r="N376"/>
       <c r="O376"/>
       <c r="P376"/>
       <c r="Q376"/>
@@ -31074,14 +31036,14 @@
       <c r="G377"/>
       <c r="H377"/>
       <c r="I377"/>
-      <c r="J377" t="s">
-        <v>26</v>
-      </c>
+      <c r="J377"/>
       <c r="K377"/>
       <c r="L377"/>
       <c r="M377"/>
       <c r="N377"/>
-      <c r="O377"/>
+      <c r="O377" t="s">
+        <v>88</v>
+      </c>
       <c r="P377"/>
       <c r="Q377"/>
       <c r="R377"/>
@@ -31099,16 +31061,16 @@
       <c r="E378"/>
       <c r="F378"/>
       <c r="G378"/>
-      <c r="H378"/>
+      <c r="H378" t="s">
+        <v>26</v>
+      </c>
       <c r="I378"/>
       <c r="J378"/>
       <c r="K378"/>
       <c r="L378"/>
       <c r="M378"/>
       <c r="N378"/>
-      <c r="O378" t="s">
-        <v>88</v>
-      </c>
+      <c r="O378"/>
       <c r="P378"/>
       <c r="Q378"/>
       <c r="R378"/>
@@ -31124,11 +31086,11 @@
       <c r="C379"/>
       <c r="D379"/>
       <c r="E379"/>
-      <c r="F379"/>
+      <c r="F379" t="s">
+        <v>26</v>
+      </c>
       <c r="G379"/>
-      <c r="H379" t="s">
-        <v>26</v>
-      </c>
+      <c r="H379"/>
       <c r="I379"/>
       <c r="J379"/>
       <c r="K379"/>
@@ -31151,16 +31113,16 @@
       <c r="C380"/>
       <c r="D380"/>
       <c r="E380"/>
-      <c r="F380" t="s">
-        <v>26</v>
-      </c>
+      <c r="F380"/>
       <c r="G380"/>
       <c r="H380"/>
       <c r="I380"/>
       <c r="J380"/>
       <c r="K380"/>
       <c r="L380"/>
-      <c r="M380"/>
+      <c r="M380" t="s">
+        <v>29</v>
+      </c>
       <c r="N380"/>
       <c r="O380"/>
       <c r="P380"/>
@@ -31182,12 +31144,12 @@
       <c r="G381"/>
       <c r="H381"/>
       <c r="I381"/>
-      <c r="J381"/>
+      <c r="J381" t="s">
+        <v>29</v>
+      </c>
       <c r="K381"/>
       <c r="L381"/>
-      <c r="M381" t="s">
-        <v>29</v>
-      </c>
+      <c r="M381"/>
       <c r="N381"/>
       <c r="O381"/>
       <c r="P381"/>
@@ -31207,11 +31169,11 @@
       <c r="E382"/>
       <c r="F382"/>
       <c r="G382"/>
-      <c r="H382"/>
+      <c r="H382" t="s">
+        <v>26</v>
+      </c>
       <c r="I382"/>
-      <c r="J382" t="s">
-        <v>29</v>
-      </c>
+      <c r="J382"/>
       <c r="K382"/>
       <c r="L382"/>
       <c r="M382"/>
@@ -31261,11 +31223,11 @@
       <c r="E384"/>
       <c r="F384"/>
       <c r="G384"/>
-      <c r="H384" t="s">
-        <v>26</v>
-      </c>
+      <c r="H384"/>
       <c r="I384"/>
-      <c r="J384"/>
+      <c r="J384" t="s">
+        <v>88</v>
+      </c>
       <c r="K384"/>
       <c r="L384"/>
       <c r="M384"/>
@@ -31315,11 +31277,11 @@
       <c r="E386"/>
       <c r="F386"/>
       <c r="G386"/>
-      <c r="H386"/>
+      <c r="H386" t="s">
+        <v>26</v>
+      </c>
       <c r="I386"/>
-      <c r="J386" t="s">
-        <v>88</v>
-      </c>
+      <c r="J386"/>
       <c r="K386"/>
       <c r="L386"/>
       <c r="M386"/>
@@ -31359,33 +31321,6 @@
       <c r="T387"/>
       <c r="U387"/>
     </row>
-    <row r="388">
-      <c r="A388" t="s">
-        <v>423</v>
-      </c>
-      <c r="B388"/>
-      <c r="C388"/>
-      <c r="D388"/>
-      <c r="E388"/>
-      <c r="F388"/>
-      <c r="G388"/>
-      <c r="H388" t="s">
-        <v>26</v>
-      </c>
-      <c r="I388"/>
-      <c r="J388"/>
-      <c r="K388"/>
-      <c r="L388"/>
-      <c r="M388"/>
-      <c r="N388"/>
-      <c r="O388"/>
-      <c r="P388"/>
-      <c r="Q388"/>
-      <c r="R388"/>
-      <c r="S388"/>
-      <c r="T388"/>
-      <c r="U388"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>